<commit_message>
stingray and pneunet rendering data generation
</commit_message>
<xml_diff>
--- a/experiments/pneunet/quarter_circle_with_gravity.xlsx
+++ b/experiments/pneunet/quarter_circle_with_gravity.xlsx
@@ -129,13 +129,13 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>0.039999242090380693</v>
+        <v>0.039999187865431982</v>
       </c>
       <c r="B7" s="0">
-        <v>0.039999840756277938</v>
+        <v>0.039998641669755503</v>
       </c>
       <c r="C7" s="0">
-        <v>0.040000261567970659</v>
+        <v>0.039997767266149668</v>
       </c>
     </row>
     <row r="8">
@@ -151,24 +151,24 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>-0.00022938093213070626</v>
+        <v>-0.00018632290153293635</v>
       </c>
       <c r="B9" s="0">
-        <v>-0.00016929902459207139</v>
+        <v>-0.00023783135019860396</v>
       </c>
       <c r="C9" s="0">
-        <v>-0.00010873898862059922</v>
+        <v>-0.00030255222421157426</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>0.059995763935999299</v>
+        <v>0.059996025808309206</v>
       </c>
       <c r="B10" s="0">
-        <v>0.059998251166121577</v>
+        <v>0.059993361105477691</v>
       </c>
       <c r="C10" s="0">
-        <v>0.05999997740382839</v>
+        <v>0.059989069200822649</v>
       </c>
     </row>
     <row r="11">
@@ -184,24 +184,24 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>-0.00063115667893927623</v>
+        <v>-0.00054507981869461293</v>
       </c>
       <c r="B12" s="0">
-        <v>-0.0004623501846355706</v>
+        <v>-0.00069981678168456985</v>
       </c>
       <c r="C12" s="0">
-        <v>-0.0002921939998735158</v>
+        <v>-0.00089423182861944747</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>0.079989350639285139</v>
+        <v>0.079989361096605038</v>
       </c>
       <c r="B13" s="0">
-        <v>0.079995199964067787</v>
+        <v>0.079982063047464275</v>
       </c>
       <c r="C13" s="0">
-        <v>0.079999204974113808</v>
+        <v>0.079970237185987697</v>
       </c>
     </row>
     <row r="14">
@@ -217,24 +217,24 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>-0.0011591767320848581</v>
+        <v>-0.0010635202827221262</v>
       </c>
       <c r="B15" s="0">
-        <v>-0.00084226988466279396</v>
+        <v>-0.0013736367375571123</v>
       </c>
       <c r="C15" s="0">
-        <v>-0.00052281599623940416</v>
+        <v>-0.0017632353838712756</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>0.099980392438658458</v>
+        <v>0.099978309772688248</v>
       </c>
       <c r="B16" s="0">
-        <v>0.099990984450842896</v>
+        <v>0.099962984829389853</v>
       </c>
       <c r="C16" s="0">
-        <v>0.099998130369754468</v>
+        <v>0.099937998877414488</v>
       </c>
     </row>
     <row r="17">
@@ -250,24 +250,24 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>-0.0017760752043533179</v>
+        <v>-0.0017299803856055018</v>
       </c>
       <c r="B18" s="0">
-        <v>-0.0012791946923679284</v>
+        <v>-0.0022482827383885399</v>
       </c>
       <c r="C18" s="0">
-        <v>-0.00077830103745195865</v>
+        <v>-0.0028993414089715256</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>0.11996953898712738</v>
+        <v>0.11996220475933851</v>
       </c>
       <c r="B19" s="0">
-        <v>0.11998602463802562</v>
+        <v>0.11993462621331887</v>
       </c>
       <c r="C19" s="0">
-        <v>0.11999696760678501</v>
+        <v>0.11988937792597402</v>
       </c>
     </row>
     <row r="20">
@@ -283,24 +283,24 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>-0.0024516014323730157</v>
+        <v>-0.0025338341012797246</v>
       </c>
       <c r="B21" s="0">
-        <v>-0.0017489473518744758</v>
+        <v>-0.0033140139524611241</v>
       </c>
       <c r="C21" s="0">
-        <v>-0.0010405945306536603</v>
+        <v>-0.0042938735303691931</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>0.13995750263234694</v>
+        <v>0.13994055144399525</v>
       </c>
       <c r="B22" s="0">
-        <v>0.13998074896470511</v>
+        <v>0.13989568786878934</v>
       </c>
       <c r="C22" s="0">
-        <v>0.13999590563065528</v>
+        <v>0.1398216033687685</v>
       </c>
     </row>
     <row r="23">
@@ -316,24 +316,24 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>-0.0031612654141537347</v>
+        <v>-0.0034654479871196013</v>
       </c>
       <c r="B24" s="0">
-        <v>-0.0022319558119206226</v>
+        <v>-0.0045623173694999478</v>
       </c>
       <c r="C24" s="0">
-        <v>-0.0012950851677379243</v>
+        <v>-0.0059396669319342014</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>0.1599449529700373</v>
+        <v>0.15991298967817913</v>
       </c>
       <c r="B25" s="0">
-        <v>0.15997553554573554</v>
+        <v>0.1598450171128547</v>
       </c>
       <c r="C25" s="0">
-        <v>0.15999508370151327</v>
+        <v>0.1597320267945799</v>
       </c>
     </row>
     <row r="26">
@@ -349,24 +349,24 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>-0.0038852406599317064</v>
+        <v>-0.0045161393889021411</v>
       </c>
       <c r="B27" s="0">
-        <v>-0.0027123782456488737</v>
+        <v>-0.0059858718565799496</v>
       </c>
       <c r="C27" s="0">
-        <v>-0.0015299528640255937</v>
+        <v>-0.0078310385654583262</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>0.1799324661671331</v>
+        <v>0.17987926125479006</v>
       </c>
       <c r="B28" s="0">
-        <v>0.17997068628796387</v>
+        <v>0.17978155966307771</v>
       </c>
       <c r="C28" s="0">
-        <v>0.17999458312810607</v>
+        <v>0.1796180455232215</v>
       </c>
     </row>
     <row r="29">
@@ -382,24 +382,24 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>-0.0046074764143619815</v>
+        <v>-0.005678138212658476</v>
       </c>
       <c r="B30" s="0">
-        <v>-0.0031773952915947028</v>
+        <v>-0.0075785162816909436</v>
       </c>
       <c r="C30" s="0">
-        <v>-0.0017356415874398745</v>
+        <v>-0.0099637614309225596</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>0.19992050620083168</v>
+        <v>0.19983918203648199</v>
       </c>
       <c r="B31" s="0">
-        <v>0.19996641978181695</v>
+        <v>0.19970431627180585</v>
       </c>
       <c r="C31" s="0">
-        <v>0.19999442796292524</v>
+        <v>0.19947703015030882</v>
       </c>
     </row>
     <row r="32">
@@ -415,24 +415,24 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>-0.0053149796853439041</v>
+        <v>-0.0069445522828732471</v>
       </c>
       <c r="B33" s="0">
-        <v>-0.0036166378486434262</v>
+        <v>-0.0093352218184543541</v>
       </c>
       <c r="C33" s="0">
-        <v>-0.001904433447856984</v>
+        <v>-0.012335043102301666</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>0.21990942388556539</v>
+        <v>0.2197926180046538</v>
       </c>
       <c r="B34" s="0">
-        <v>0.21996287433357392</v>
+        <v>0.21961230320829944</v>
       </c>
       <c r="C34" s="0">
-        <v>0.21999459020997061</v>
+        <v>0.21930625489760067</v>
       </c>
     </row>
     <row r="35">
@@ -448,24 +448,24 @@
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>-0.0059972347937270985</v>
+        <v>-0.00830933627501859</v>
       </c>
       <c r="B36" s="0">
-        <v>-0.0040217247042700277</v>
+        <v>-0.011252068489995014</v>
       </c>
       <c r="C36" s="0">
-        <v>-0.0020301049261905939</v>
+        <v>-0.01494350856068782</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>0.23989946510047822</v>
+        <v>0.23973946458190049</v>
       </c>
       <c r="B37" s="0">
-        <v>0.23996011595374811</v>
+        <v>0.23950451563620795</v>
       </c>
       <c r="C37" s="0">
-        <v>0.23999499693958234</v>
+        <v>0.23910282927463575</v>
       </c>
     </row>
     <row r="38">
@@ -481,24 +481,24 @@
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>-0.0066457342387889664</v>
+        <v>-0.0097672641887652459</v>
       </c>
       <c r="B39" s="0">
-        <v>-0.0043858891775528921</v>
+        <v>-0.013326225967040032</v>
       </c>
       <c r="C39" s="0">
-        <v>-0.0021076498083758182</v>
+        <v>-0.017789187295421598</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>0.2598907831193692</v>
+        <v>0.25967962865211502</v>
       </c>
       <c r="B40" s="0">
-        <v>0.25995814827801089</v>
+        <v>0.25937989299829051</v>
       </c>
       <c r="C40" s="0">
-        <v>0.25999553784795065</v>
+        <v>0.25886362960040205</v>
       </c>
     </row>
     <row r="41">
@@ -514,24 +514,24 @@
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>-0.0072535996768534018</v>
+        <v>-0.011313905314234306</v>
       </c>
       <c r="B42" s="0">
-        <v>-0.0047036779657501004</v>
+        <v>-0.015555938601613809</v>
       </c>
       <c r="C42" s="0">
-        <v>-0.0021330563918922881</v>
+        <v>-0.020873504539756296</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>0.27988345212000465</v>
+        <v>0.27961301276283168</v>
       </c>
       <c r="B43" s="0">
-        <v>0.27995692273482947</v>
+        <v>0.27923728556890853</v>
       </c>
       <c r="C43" s="0">
-        <v>0.27999607249787328</v>
+        <v>0.27858522895489007</v>
       </c>
     </row>
     <row r="44">
@@ -547,24 +547,24 @@
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>-0.007815275891302707</v>
+        <v>-0.012945603635589826</v>
       </c>
       <c r="B45" s="0">
-        <v>-0.0049707086453367978</v>
+        <v>-0.017940514650365533</v>
       </c>
       <c r="C45" s="0">
-        <v>-0.0021031289770737987</v>
+        <v>-0.024199276414790472</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>0.29987748028707195</v>
+        <v>0.29953950104476296</v>
       </c>
       <c r="B46" s="0">
-        <v>0.29995634808937016</v>
+        <v>0.2990754213683402</v>
       </c>
       <c r="C46" s="0">
-        <v>0.29999643689677946</v>
+        <v>0.29826382413040553</v>
       </c>
     </row>
     <row r="47">
@@ -580,24 +580,24 @@
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>-0.0083262839469167727</v>
+        <v>-0.014659460612705691</v>
       </c>
       <c r="B48" s="0">
-        <v>-0.0051834749302780599</v>
+        <v>-0.020480319618094621</v>
       </c>
       <c r="C48" s="0">
-        <v>-0.0020153456489681995</v>
+        <v>-0.027770708658621295</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>0.31987282173043968</v>
+        <v>0.31945894642461042</v>
       </c>
       <c r="B49" s="0">
-        <v>0.3199562989799471</v>
+        <v>0.31889287265194305</v>
       </c>
       <c r="C49" s="0">
-        <v>0.31999644931363619</v>
+        <v>0.3178951581324192</v>
       </c>
     </row>
     <row r="50">
@@ -613,24 +613,24 @@
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>-0.008783022409226347</v>
+        <v>-0.016453321281413427</v>
       </c>
       <c r="B51" s="0">
-        <v>-0.0053391909477320237</v>
+        <v>-0.023176773630162736</v>
       </c>
       <c r="C51" s="0">
-        <v>-0.0018677459871196723</v>
+        <v>-0.031593398511536988</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>0.33986938691546353</v>
+        <v>0.33937115873981372</v>
       </c>
       <c r="B52" s="0">
-        <v>0.33995662334557225</v>
+        <v>0.3386880211920536</v>
       </c>
       <c r="C52" s="0">
-        <v>0.33999591537559565</v>
+        <v>0.33747443674069888</v>
       </c>
     </row>
     <row r="53">
@@ -646,24 +646,24 @@
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>-0.0091826076892688267</v>
+        <v>-0.018325763615001014</v>
       </c>
       <c r="B54" s="0">
-        <v>-0.005435667551204411</v>
+        <v>-0.026032352720070363</v>
       </c>
       <c r="C54" s="0">
-        <v>-0.0016588436841866703</v>
+        <v>-0.035674339207031544</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>0.35986705157128196</v>
+        <v>0.35927589338852084</v>
       </c>
       <c r="B55" s="0">
-        <v>0.35995714880024765</v>
+        <v>0.35845902156159937</v>
       </c>
       <c r="C55" s="0">
-        <v>0.35999463256102709</v>
+        <v>0.35699623758501825</v>
       </c>
     </row>
     <row r="56">
@@ -679,24 +679,24 @@
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>-0.0095227463447374022</v>
+        <v>-0.020276091093393782</v>
       </c>
       <c r="B57" s="0">
-        <v>-0.0054712151334828877</v>
+        <v>-0.029050593893449269</v>
       </c>
       <c r="C57" s="0">
-        <v>-0.0013875601708565831</v>
+        <v>-0.040021926376570191</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>0.37986566418684026</v>
+        <v>0.37917284016516595</v>
       </c>
       <c r="B58" s="0">
-        <v>0.37995768809182856</v>
+        <v>0.37820376160591584</v>
       </c>
       <c r="C58" s="0">
-        <v>0.3799923942449881</v>
+        <v>0.37645441011785696</v>
       </c>
     </row>
     <row r="59">
@@ -712,24 +712,24 @@
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>-0.00980163361135491</v>
+        <v>-0.022304328431130768</v>
       </c>
       <c r="B60" s="0">
-        <v>-0.0054445685924272118</v>
+        <v>-0.032236103799952565</v>
       </c>
       <c r="C60" s="0">
-        <v>-0.0010531762848527877</v>
+        <v>-0.044645965506890602</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0">
-        <v>0.39986505227363839</v>
+        <v>0.39906161194198236</v>
       </c>
       <c r="B61" s="0">
-        <v>0.3999580438222784</v>
+        <v>0.39791981925336101</v>
       </c>
       <c r="C61" s="0">
-        <v>0.39998899347322814</v>
+        <v>0.39584196478190409</v>
       </c>
     </row>
     <row r="62">
@@ -745,24 +745,24 @@
     </row>
     <row r="63">
       <c r="A63" s="0">
-        <v>-0.010017873619912679</v>
+        <v>-0.024411220420257337</v>
       </c>
       <c r="B63" s="0">
-        <v>-0.0053548310963551383</v>
+        <v>-0.035594570807750608</v>
       </c>
       <c r="C63" s="0">
-        <v>-0.0006552998286525805</v>
+        <v>-0.049557679385005361</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0">
-        <v>0.41986502760080929</v>
+        <v>0.41894173285978631</v>
       </c>
       <c r="B64" s="0">
-        <v>0.41995801262174298</v>
+        <v>0.41760441476609428</v>
       </c>
       <c r="C64" s="0">
-        <v>0.41998422665200746</v>
+        <v>0.41515094957654236</v>
       </c>
     </row>
     <row r="65">
@@ -778,24 +778,24 @@
     </row>
     <row r="66">
       <c r="A66" s="0">
-        <v>-0.010170417729237942</v>
+        <v>-0.026598233849039209</v>
       </c>
       <c r="B66" s="0">
-        <v>-0.0052014341377102404</v>
+        <v>-0.03913278022907709</v>
       </c>
       <c r="C66" s="0">
-        <v>-0.00019384757040053058</v>
+        <v>-0.05476971421991076</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0">
-        <v>0.43986539061189228</v>
+        <v>0.43881262568756579</v>
       </c>
       <c r="B67" s="0">
-        <v>0.43995738897333525</v>
+        <v>0.4372543574699263</v>
       </c>
       <c r="C67" s="0">
-        <v>0.43997789734977133</v>
+        <v>0.43437231212988453</v>
       </c>
     </row>
     <row r="68">
@@ -811,24 +811,24 @@
     </row>
     <row r="69">
       <c r="A69" s="0">
-        <v>-0.010258518218170809</v>
+        <v>-0.028867562461433252</v>
       </c>
       <c r="B69" s="0">
-        <v>-0.004984112092245239</v>
+        <v>-0.042858632386706799</v>
       </c>
       <c r="C69" s="0">
-        <v>0.0003309591124960977</v>
+        <v>-0.060296142832222809</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0">
-        <v>0.45986593422571481</v>
+        <v>0.45867359799982099</v>
       </c>
       <c r="B70" s="0">
-        <v>0.4599559688862791</v>
+        <v>0.4568659859266252</v>
       </c>
       <c r="C70" s="0">
-        <v>0.45996982041675594</v>
+        <v>0.45349574528829589</v>
       </c>
     </row>
     <row r="71">
@@ -844,24 +844,24 @@
     </row>
     <row r="72">
       <c r="A72" s="0">
-        <v>-0.010281695267629398</v>
+        <v>-0.031222134924985177</v>
       </c>
       <c r="B72" s="0">
-        <v>-0.0047028901491518327</v>
+        <v>-0.046781163137155461</v>
       </c>
       <c r="C72" s="0">
-        <v>0.00091858513834631539</v>
+        <v>-0.066152462943357623</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0">
-        <v>0.47986644721344485</v>
+        <v>0.47852382680314975</v>
       </c>
       <c r="B73" s="0">
-        <v>0.47995355361648256</v>
+        <v>0.47643510042380177</v>
       </c>
       <c r="C73" s="0">
-        <v>0.47995982664174486</v>
+        <v>0.47250951415307091</v>
       </c>
     </row>
     <row r="74">
@@ -877,24 +877,24 @@
     </row>
     <row r="75">
       <c r="A75" s="0">
-        <v>-0.010239715758358069</v>
+        <v>-0.033665625775684153</v>
       </c>
       <c r="B75" s="0">
-        <v>-0.0043580850747363311</v>
+        <v>-0.050910566373012091</v>
       </c>
       <c r="C75" s="0">
-        <v>0.0015681587649742305</v>
+        <v>-0.072355588163096077</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0">
-        <v>0.49986671733443921</v>
+        <v>0.49836234121906942</v>
       </c>
       <c r="B76" s="0">
-        <v>0.49994995363802364</v>
+        <v>0.49595688655709186</v>
       </c>
       <c r="C76" s="0">
-        <v>0.49994776818173647</v>
+        <v>0.49140026243670665</v>
       </c>
     </row>
     <row r="77">
@@ -910,24 +910,24 @@
     </row>
     <row r="78">
       <c r="A78" s="0">
-        <v>-0.010132582937960389</v>
+        <v>-0.036202469306639042</v>
       </c>
       <c r="B78" s="0">
-        <v>-0.0039503188453425256</v>
+        <v>-0.055258217909738547</v>
       </c>
       <c r="C78" s="0">
-        <v>0.0022784337426546273</v>
+        <v>-0.078923828755966749</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0">
-        <v>0.5198665344074257</v>
+        <v>0.5181880027982575</v>
       </c>
       <c r="B79" s="0">
-        <v>0.5199449930772857</v>
+        <v>0.51542582856784969</v>
       </c>
       <c r="C79" s="0">
-        <v>0.51993352501893453</v>
+        <v>0.51015279599591257</v>
       </c>
     </row>
     <row r="80">
@@ -943,24 +943,24 @@
     </row>
     <row r="81">
       <c r="A81" s="0">
-        <v>-0.0099605364961885805</v>
+        <v>-0.038837876362503507</v>
       </c>
       <c r="B81" s="0">
-        <v>-0.0034805457601220437</v>
+        <v>-0.059836700016323893</v>
       </c>
       <c r="C81" s="0">
-        <v>0.0030477348795551638</v>
+        <v>-0.085876858649496526</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0">
-        <v>0.53986569349206293</v>
+        <v>0.5379994830019188</v>
       </c>
       <c r="B82" s="0">
-        <v>0.53993851483311261</v>
+        <v>0.53483561097863674</v>
       </c>
       <c r="C82" s="0">
-        <v>0.53991701271691972</v>
+        <v>0.52874984144737136</v>
       </c>
     </row>
     <row r="83">
@@ -976,24 +976,24 @@
     </row>
     <row r="84">
       <c r="A84" s="0">
-        <v>-0.0097240630520875476</v>
+        <v>-0.041577853992483649</v>
       </c>
       <c r="B84" s="0">
-        <v>-0.0029500942469175783</v>
+        <v>-0.064659825668289553</v>
       </c>
       <c r="C84" s="0">
-        <v>0.0038738845787230978</v>
+        <v>-0.09323566441718692</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0">
-        <v>0.55986399835941447</v>
+        <v>0.55779523733842773</v>
       </c>
       <c r="B85" s="0">
-        <v>0.55993038661937777</v>
+        <v>0.55417900694102673</v>
       </c>
       <c r="C85" s="0">
-        <v>0.55989819175776068</v>
+        <v>0.54717177791432192</v>
       </c>
     </row>
     <row r="86">
@@ -1009,24 +1009,24 @@
     </row>
     <row r="87">
       <c r="A87" s="0">
-        <v>-0.00942391752140616</v>
+        <v>-0.044429227900455184</v>
       </c>
       <c r="B87" s="0">
-        <v>-0.002360725232249112</v>
+        <v>-0.069742661378605991</v>
       </c>
       <c r="C87" s="0">
-        <v>0.0047541070498560972</v>
+        <v>-0.10102247111251393</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0">
-        <v>0.57986126543803274</v>
+        <v>0.57757347558726091</v>
       </c>
       <c r="B88" s="0">
-        <v>0.57992050817673613</v>
+        <v>0.57344775157950523</v>
       </c>
       <c r="C88" s="0">
-        <v>0.57987707873320693</v>
+        <v>0.5653963402246498</v>
       </c>
     </row>
     <row r="89">
@@ -1042,24 +1042,24 @@
     </row>
     <row r="90">
       <c r="A90" s="0">
-        <v>-0.0090611563186354434</v>
+        <v>-0.047399667609922744</v>
       </c>
       <c r="B90" s="0">
-        <v>-0.0017147096890787565</v>
+        <v>-0.075101547188861834</v>
       </c>
       <c r="C90" s="0">
-        <v>0.00568490589239535</v>
+        <v>-0.10926063883520842</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0">
-        <v>0.59985732843400985</v>
+        <v>0.59733212747701492</v>
       </c>
       <c r="B91" s="0">
-        <v>0.59990881990080891</v>
+        <v>0.59263239848707139</v>
       </c>
       <c r="C91" s="0">
-        <v>0.59985375961763021</v>
+        <v>0.58339829233186624</v>
       </c>
     </row>
     <row r="92">
@@ -1075,24 +1075,24 @@
     </row>
     <row r="93">
       <c r="A93" s="0">
-        <v>-0.008637183877041793</v>
+        <v>-0.050497714232725206</v>
       </c>
       <c r="B93" s="0">
-        <v>-0.0010149288376038214</v>
+        <v>-0.08075411207003684</v>
       </c>
       <c r="C93" s="0">
-        <v>0.0066619095421754648</v>
+        <v>-0.1179745227687037</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0">
-        <v>0.619852043836146</v>
+        <v>0.61706880310943857</v>
       </c>
       <c r="B94" s="0">
-        <v>0.61989531311242629</v>
+        <v>0.61172215741040148</v>
       </c>
       <c r="C94" s="0">
-        <v>0.61982840523809379</v>
+        <v>0.60114907041872534</v>
       </c>
     </row>
     <row r="95">
@@ -1108,24 +1108,24 @@
     </row>
     <row r="96">
       <c r="A96" s="0">
-        <v>-0.0081538145660716623</v>
+        <v>-0.053732810691651742</v>
       </c>
       <c r="B96" s="0">
-        <v>-0.00026500149436216146</v>
+        <v>-0.086719282578696641</v>
       </c>
       <c r="C96" s="0">
-        <v>0.0076796776157511543</v>
+        <v>-0.12718928813499028</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0">
-        <v>0.63984529752708863</v>
+        <v>0.63678074733642598</v>
       </c>
       <c r="B97" s="0">
-        <v>0.63988004213172978</v>
+        <v>0.63070471106593406</v>
       </c>
       <c r="C97" s="0">
-        <v>0.63980128882966247</v>
+        <v>0.61861639614280794</v>
       </c>
     </row>
     <row r="98">
@@ -1141,24 +1141,24 @@
     </row>
     <row r="99">
       <c r="A99" s="0">
-        <v>-0.0076133527755816261</v>
+        <v>-0.057115334196208192</v>
       </c>
       <c r="B99" s="0">
-        <v>0.00053055570946999289</v>
+        <v>-0.093017282128303805</v>
       </c>
       <c r="C99" s="0">
-        <v>0.0087314594062409597</v>
+        <v>-0.13693067007691834</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0">
-        <v>0.65983701272063644</v>
+        <v>0.65646478720133972</v>
       </c>
       <c r="B100" s="0">
-        <v>0.65986313817936648</v>
+        <v>0.64956600896770167</v>
       </c>
       <c r="C100" s="0">
-        <v>0.65977280514507075</v>
+        <v>0.63576386188324496</v>
       </c>
     </row>
     <row r="101">
@@ -1174,24 +1174,24 @@
     </row>
     <row r="102">
       <c r="A102" s="0">
-        <v>-0.0070186947519755372</v>
+        <v>-0.060656630704903715</v>
       </c>
       <c r="B102" s="0">
-        <v>0.0013661280316999949</v>
+        <v>-0.099669617653454404</v>
       </c>
       <c r="C102" s="0">
-        <v>0.0098088935985557024</v>
+        <v>-0.14722466691977812</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0">
-        <v>0.67982715942231875</v>
+        <v>0.67611727144963685</v>
       </c>
       <c r="B103" s="0">
-        <v>0.67984482486266884</v>
+        <v>0.66829003614288074</v>
       </c>
       <c r="C103" s="0">
-        <v>0.67974348985594246</v>
+        <v>0.65255049175325941</v>
       </c>
     </row>
     <row r="104">
@@ -1207,24 +1207,24 @@
     </row>
     <row r="105">
       <c r="A105" s="0">
-        <v>-0.0063734567498913855</v>
+        <v>-0.064369051023285703</v>
       </c>
       <c r="B105" s="0">
-        <v>0.0022347532161727753</v>
+        <v>-0.10669904975323694</v>
       </c>
       <c r="C105" s="0">
-        <v>0.010901635578255253</v>
+        <v>-0.15809715362709542</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0">
-        <v>0.69981576554505665</v>
+        <v>0.69573400099649962</v>
       </c>
       <c r="B106" s="0">
-        <v>0.69982543453010426</v>
+        <v>0.68685855468783352</v>
       </c>
       <c r="C106" s="0">
-        <v>0.69971403674760391</v>
+        <v>0.66893028467559168</v>
       </c>
     </row>
     <row r="107">
@@ -1240,24 +1240,24 @@
     </row>
     <row r="108">
       <c r="A108" s="0">
-        <v>-0.0056821352496289829</v>
+        <v>-0.068265988080530055</v>
       </c>
       <c r="B108" s="0">
-        <v>0.0031278117191449089</v>
+        <v>-0.11412954158440533</v>
       </c>
       <c r="C108" s="0">
-        <v>0.011996895383591425</v>
+        <v>-0.16957340062411438</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0">
-        <v>0.71980292967227366</v>
+        <v>0.7153101491114231</v>
       </c>
       <c r="B109" s="0">
-        <v>0.71980542396352731</v>
+        <v>0.70525081630972519</v>
       </c>
       <c r="C109" s="0">
-        <v>0.71968530817390275</v>
+        <v>0.68485174911121005</v>
       </c>
     </row>
     <row r="110">
@@ -1273,24 +1273,24 @@
     </row>
     <row r="111">
       <c r="A111" s="0">
-        <v>-0.0049503064398682727</v>
+        <v>-0.072361914793896254</v>
       </c>
       <c r="B111" s="0">
-        <v>0.0040346425464968649</v>
+        <v>-0.12198618082230504</v>
       </c>
       <c r="C111" s="0">
-        <v>0.013078865248084963</v>
+        <v>-0.18167748163271172</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0">
-        <v>0.73978883519622629</v>
+        <v>0.7348401699424153</v>
       </c>
       <c r="B112" s="0">
-        <v>0.73978538652156833</v>
+        <v>0.72344324435003604</v>
       </c>
       <c r="C112" s="0">
-        <v>0.73965833093993594</v>
+        <v>0.70025744322634509</v>
       </c>
     </row>
     <row r="113">
@@ -1306,24 +1306,24 @@
     </row>
     <row r="114">
       <c r="A114" s="0">
-        <v>-0.0041848739444473046</v>
+        <v>-0.076672421764065399</v>
       </c>
       <c r="B114" s="0">
-        <v>0.0049420672865930857</v>
+        <v>-0.13029506790648593</v>
       </c>
       <c r="C114" s="0">
-        <v>0.014128010634146759</v>
+        <v>-0.19443155291576564</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0">
-        <v>0.7597737650888009</v>
+        <v>0.75431769385739511</v>
       </c>
       <c r="B115" s="0">
-        <v>0.75976605563201471</v>
+        <v>0.74140908435142305</v>
       </c>
       <c r="C115" s="0">
-        <v>0.75963426450250915</v>
+        <v>0.71508353951332326</v>
       </c>
     </row>
     <row r="116">
@@ -1339,24 +1339,24 @@
     </row>
     <row r="117">
       <c r="A117" s="0">
-        <v>-0.0033943759631013576</v>
+        <v>-0.08121425383853248</v>
       </c>
       <c r="B117" s="0">
-        <v>0.0058338007393415299</v>
+        <v>-0.13908316253234382</v>
       </c>
       <c r="C117" s="0">
-        <v>0.015120192490937398</v>
+        <v>-0.20785498561139379</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0">
-        <v>0.77975811575848997</v>
+        <v>0.77373540793039641</v>
       </c>
       <c r="B118" s="0">
-        <v>0.77974829096448617</v>
+        <v>0.7591180230768434</v>
       </c>
       <c r="C118" s="0">
-        <v>0.77961432001362063</v>
+        <v>0.72925943925564907</v>
       </c>
     </row>
     <row r="119">
@@ -1372,24 +1372,24 @@
     </row>
     <row r="120">
       <c r="A120" s="0">
-        <v>-0.002589365699048394</v>
+        <v>-0.086005344326873151</v>
       </c>
       <c r="B120" s="0">
-        <v>0.0066897214074171088</v>
+        <v>-0.14837807894158248</v>
       </c>
       <c r="C120" s="0">
-        <v>0.016025581029768528</v>
+        <v>-0.22196333298077089</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0">
-        <v>0.79974240711194977</v>
+        <v>0.79308491974973694</v>
       </c>
       <c r="B121" s="0">
-        <v>0.79973303293636122</v>
+        <v>0.77653577710337895</v>
       </c>
       <c r="C121" s="0">
-        <v>0.79959959557859217</v>
+        <v>0.74270746980007418</v>
       </c>
     </row>
     <row r="122">
@@ -1405,24 +1405,24 @@
     </row>
     <row r="123">
       <c r="A123" s="0">
-        <v>-0.0017828822813705004</v>
+        <v>-0.091064845341612008</v>
       </c>
       <c r="B123" s="0">
-        <v>0.0074849688653576977</v>
+        <v>-0.15820781901700645</v>
       </c>
       <c r="C123" s="0">
-        <v>0.01680731254485111</v>
+        <v>-0.23676711583476212</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0">
-        <v>0.81972728376190607</v>
+        <v>0.8123566025808624</v>
       </c>
       <c r="B124" s="0">
-        <v>0.81972120224229983</v>
+        <v>0.79362365379304978</v>
       </c>
       <c r="C124" s="0">
-        <v>0.81959077255172397</v>
+        <v>0.75534270632138079</v>
       </c>
     </row>
     <row r="125">
@@ -1438,24 +1438,24 @@
     </row>
     <row r="126">
       <c r="A126" s="0">
-        <v>-0.00099103349839607885</v>
+        <v>-0.096413152360956295</v>
       </c>
       <c r="B126" s="0">
-        <v>0.0081888275267844347</v>
+        <v>-0.16860043053422838</v>
       </c>
       <c r="C126" s="0">
-        <v>0.017419830923757488</v>
+        <v>-0.25227041269720801</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0">
-        <v>0.83971349882505952</v>
+        <v>0.83153941978732027</v>
       </c>
       <c r="B127" s="0">
-        <v>0.83971350705124492</v>
+        <v>0.81033808970602761</v>
       </c>
       <c r="C127" s="0">
-        <v>0.8395875857892553</v>
+        <v>0.76707296943455816</v>
       </c>
     </row>
     <row r="128">
@@ -1471,24 +1471,24 @@
     </row>
     <row r="129">
       <c r="A129" s="0">
-        <v>-0.00023371669759137214</v>
+        <v>-0.10207192065278624</v>
       </c>
       <c r="B129" s="0">
-        <v>0.008763347581900692</v>
+        <v>-0.17958357622452514</v>
       </c>
       <c r="C129" s="0">
-        <v>0.017806845291212223</v>
+        <v>-0.26846924707515674</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0">
-        <v>0.85970186619186384</v>
+        <v>0.850620726312041</v>
       </c>
       <c r="B130" s="0">
-        <v>0.85971009863739367</v>
+        <v>0.82663017449989851</v>
       </c>
       <c r="C130" s="0">
-        <v>0.85958793157388758</v>
+        <v>0.77779906018622846</v>
       </c>
     </row>
     <row r="131">
@@ -1504,24 +1504,24 @@
     </row>
     <row r="132">
       <c r="A132" s="0">
-        <v>0.00046448966240673109</v>
+        <v>-0.10806407064962807</v>
       </c>
       <c r="B132" s="0">
-        <v>0.0091616441734212496</v>
+        <v>-0.19118399765724936</v>
       </c>
       <c r="C132" s="0">
-        <v>0.017898826769108776</v>
+        <v>-0.28534977330454181</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0">
-        <v>0.87969315838153439</v>
+        <v>0.86958604496514547</v>
       </c>
       <c r="B133" s="0">
-        <v>0.87970998234325248</v>
+        <v>0.84244517219374759</v>
       </c>
       <c r="C133" s="0">
-        <v>0.87958640164316904</v>
+        <v>0.78741530388334091</v>
       </c>
     </row>
     <row r="134">
@@ -1537,24 +1537,24 @@
     </row>
     <row r="135">
       <c r="A135" s="0">
-        <v>0.0010732239769347157</v>
+        <v>-0.11441377870737503</v>
       </c>
       <c r="B135" s="0">
-        <v>0.0093258061901228869</v>
+        <v>-0.20342685650560333</v>
       </c>
       <c r="C135" s="0">
-        <v>0.01760996522654687</v>
+        <v>-0.30288627563724407</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0">
-        <v>0.89968791336720944</v>
+        <v>0.88841881527711142</v>
       </c>
       <c r="B136" s="0">
-        <v>0.8997100386913518</v>
+        <v>0.85772205650982547</v>
       </c>
       <c r="C136" s="0">
-        <v>0.89957191784855206</v>
+        <v>0.79581048271720578</v>
       </c>
     </row>
     <row r="137">
@@ -1570,24 +1570,24 @@
     </row>
     <row r="138">
       <c r="A138" s="0">
-        <v>0.0015549805825952839</v>
+        <v>-0.12114644890109756</v>
       </c>
       <c r="B138" s="0">
-        <v>0.0091843387614222866</v>
+        <v>-0.21633493473102702</v>
       </c>
       <c r="C138" s="0">
-        <v>0.0168345207881169</v>
+        <v>-0.32103901329898182</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0">
-        <v>0.91968609239371846</v>
+        <v>0.9071001127878906</v>
       </c>
       <c r="B139" s="0">
-        <v>0.91970343004638688</v>
+        <v>0.87239308296396589</v>
       </c>
       <c r="C139" s="0">
-        <v>0.9195239724805947</v>
+        <v>0.8028692425401931</v>
       </c>
     </row>
     <row r="140">
@@ -1603,24 +1603,24 @@
     </row>
     <row r="141">
       <c r="A141" s="0">
-        <v>0.0018634320802138691</v>
+        <v>-0.12828866059437791</v>
       </c>
       <c r="B141" s="0">
-        <v>0.0086490638415659508</v>
+        <v>-0.22992767490681559</v>
       </c>
       <c r="C141" s="0">
-        <v>0.015442554116560101</v>
+        <v>-0.33975196774349148</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0">
-        <v>0.93968649776746793</v>
+        <v>0.92560833689323574</v>
       </c>
       <c r="B142" s="0">
-        <v>0.9396770485682655</v>
+        <v>0.88638342754185395</v>
       </c>
       <c r="C142" s="0">
-        <v>0.93940673376586681</v>
+        <v>0.80847405923101701</v>
       </c>
     </row>
     <row r="143">
@@ -1636,24 +1636,24 @@
     </row>
     <row r="144">
       <c r="A144" s="0">
-        <v>0.0019413675355449095</v>
+        <v>-0.13586808545062387</v>
       </c>
       <c r="B144" s="0">
-        <v>0.0076114219222574034</v>
+        <v>-0.24422004269867625</v>
       </c>
       <c r="C144" s="0">
-        <v>0.013275141601573386</v>
+        <v>-0.35895057739786429</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0">
-        <v>0.95968580882689425</v>
+        <v>0.94391886580986351</v>
       </c>
       <c r="B145" s="0">
-        <v>0.95960748413034103</v>
+        <v>0.89961093017408567</v>
       </c>
       <c r="C145" s="0">
-        <v>0.95915993633422825</v>
+        <v>0.81250784211105254</v>
       </c>
     </row>
     <row r="146">
@@ -1669,24 +1669,24 @@
     </row>
     <row r="147">
       <c r="A147" s="0">
-        <v>0.0017181720589075627</v>
+        <v>-0.14391336632558699</v>
       </c>
       <c r="B147" s="0">
-        <v>0.0059381762204356106</v>
+        <v>-0.25922119594031773</v>
       </c>
       <c r="C147" s="0">
-        <v>0.010139446933987243</v>
+        <v>-0.37853957925305048</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0">
-        <v>0.97967701694400788</v>
+        <v>0.96200367791518127</v>
       </c>
       <c r="B148" s="0">
-        <v>0.97945473645754944</v>
+        <v>0.91198599067734964</v>
       </c>
       <c r="C148" s="0">
-        <v>0.97868504535420808</v>
+        <v>0.81485723277199784</v>
       </c>
     </row>
     <row r="149">
@@ -1702,24 +1702,24 @@
     </row>
     <row r="150">
       <c r="A150" s="0">
-        <v>0.001106773500629783</v>
+        <v>-0.15245394908595064</v>
       </c>
       <c r="B150" s="0">
-        <v>0.0034666595935350535</v>
+        <v>-0.27493294941687119</v>
       </c>
       <c r="C150" s="0">
-        <v>0.0058045557947844287</v>
+        <v>-0.39840111403823814</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0">
-        <v>0.99964692392347665</v>
+        <v>0.97983093974438551</v>
       </c>
       <c r="B151" s="0">
-        <v>0.99915254834226774</v>
+        <v>0.92341167502774724</v>
       </c>
       <c r="C151" s="0">
-        <v>0.99782473301216279</v>
+        <v>0.81541662438072182</v>
       </c>
     </row>
     <row r="152">
@@ -1735,13 +1735,13 @@
     </row>
     <row r="153">
       <c r="A153" s="0">
-        <v>0</v>
+        <v>-0.1615198568459128</v>
       </c>
       <c r="B153" s="0">
-        <v>0</v>
+        <v>-0.29134803213847932</v>
       </c>
       <c r="C153" s="0">
-        <v>0</v>
+        <v>-0.41839328931791631</v>
       </c>
     </row>
     <row r="154">

</xml_diff>

<commit_message>
added rod contact with ground example
</commit_message>
<xml_diff>
--- a/experiments/pneunet/quarter_circle_with_gravity.xlsx
+++ b/experiments/pneunet/quarter_circle_with_gravity.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -52,13 +52,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C203"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="16.42578125" customWidth="true"/>
     <col min="2" max="2" width="16.42578125" customWidth="true"/>
-    <col min="1" max="1" width="16.42578125" customWidth="true"/>
+    <col min="1" max="1" width="15.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -129,7 +132,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>0.039999187865431982</v>
+        <v>0.040000393448394019</v>
       </c>
       <c r="B7" s="0">
         <v>0.039998641669755503</v>
@@ -151,7 +154,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>-0.00018632290153293635</v>
+        <v>8.0904185094077174e-05</v>
       </c>
       <c r="B9" s="0">
         <v>-0.00023783135019860396</v>
@@ -162,7 +165,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>0.059996025808309206</v>
+        <v>0.060000402724620663</v>
       </c>
       <c r="B10" s="0">
         <v>0.059993361105477691</v>
@@ -184,7 +187,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>-0.00054507981869461293</v>
+        <v>0.00022893671078018558</v>
       </c>
       <c r="B12" s="0">
         <v>-0.00069981678168456985</v>
@@ -195,7 +198,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>0.079989361096605038</v>
+        <v>0.079999919458515353</v>
       </c>
       <c r="B13" s="0">
         <v>0.079982063047464275</v>
@@ -217,7 +220,7 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>-0.0010635202827221262</v>
+        <v>0.0004329364119163195</v>
       </c>
       <c r="B15" s="0">
         <v>-0.0013736367375571123</v>
@@ -228,7 +231,7 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>0.099978309772688248</v>
+        <v>0.099998902518024999</v>
       </c>
       <c r="B16" s="0">
         <v>0.099962984829389853</v>
@@ -250,7 +253,7 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>-0.0017299803856055018</v>
+        <v>0.00068385998607482616</v>
       </c>
       <c r="B18" s="0">
         <v>-0.0022482827383885399</v>
@@ -261,7 +264,7 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>0.11996220475933851</v>
+        <v>0.11999734958525113</v>
       </c>
       <c r="B19" s="0">
         <v>0.11993462621331887</v>
@@ -283,7 +286,7 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>-0.0025338341012797246</v>
+        <v>0.00097437919335646695</v>
       </c>
       <c r="B21" s="0">
         <v>-0.0033140139524611241</v>
@@ -294,7 +297,7 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>0.13994055144399525</v>
+        <v>0.13999527941231149</v>
       </c>
       <c r="B22" s="0">
         <v>0.13989568786878934</v>
@@ -316,7 +319,7 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>-0.0034654479871196013</v>
+        <v>0.001298554321017023</v>
       </c>
       <c r="B24" s="0">
         <v>-0.0045623173694999478</v>
@@ -327,7 +330,7 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>0.15991298967817913</v>
+        <v>0.15999272093643743</v>
       </c>
       <c r="B25" s="0">
         <v>0.1598450171128547</v>
@@ -349,7 +352,7 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>-0.0045161393889021411</v>
+        <v>0.0016515694584630218</v>
       </c>
       <c r="B27" s="0">
         <v>-0.0059858718565799496</v>
@@ -360,7 +363,7 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>0.17987926125479006</v>
+        <v>0.17998970677200701</v>
       </c>
       <c r="B28" s="0">
         <v>0.17978155966307771</v>
@@ -382,7 +385,7 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>-0.005678138212658476</v>
+        <v>0.0020295178313289712</v>
       </c>
       <c r="B30" s="0">
         <v>-0.0075785162816909436</v>
@@ -393,7 +396,7 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>0.19983918203648199</v>
+        <v>0.19998626947172521</v>
       </c>
       <c r="B31" s="0">
         <v>0.19970431627180585</v>
@@ -415,7 +418,7 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>-0.0069445522828732471</v>
+        <v>0.0024292276486627255</v>
       </c>
       <c r="B33" s="0">
         <v>-0.0093352218184543541</v>
@@ -426,7 +429,7 @@
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>0.2197926180046538</v>
+        <v>0.21998243951985058</v>
       </c>
       <c r="B34" s="0">
         <v>0.21961230320829944</v>
@@ -448,7 +451,7 @@
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>-0.00830933627501859</v>
+        <v>0.0028481207103325779</v>
       </c>
       <c r="B36" s="0">
         <v>-0.011252068489995014</v>
@@ -459,7 +462,7 @@
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>0.23973946458190049</v>
+        <v>0.23997824439218543</v>
       </c>
       <c r="B37" s="0">
         <v>0.23950451563620795</v>
@@ -481,7 +484,7 @@
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>-0.0097672641887652459</v>
+        <v>0.0032840974759685551</v>
       </c>
       <c r="B39" s="0">
         <v>-0.013326225967040032</v>
@@ -492,7 +495,7 @@
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>0.25967962865211502</v>
+        <v>0.2599737082593247</v>
       </c>
       <c r="B40" s="0">
         <v>0.25937989299829051</v>
@@ -514,7 +517,7 @@
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>-0.011313905314234306</v>
+        <v>0.0037354434734995414</v>
       </c>
       <c r="B42" s="0">
         <v>-0.015555938601613809</v>
@@ -525,7 +528,7 @@
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>0.27961301276283168</v>
+        <v>0.27996885206651662</v>
       </c>
       <c r="B43" s="0">
         <v>0.27923728556890853</v>
@@ -547,7 +550,7 @@
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>-0.012945603635589826</v>
+        <v>0.0042007528753908296</v>
       </c>
       <c r="B45" s="0">
         <v>-0.017940514650365533</v>
@@ -558,7 +561,7 @@
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>0.29953950104476296</v>
+        <v>0.29996369382498672</v>
       </c>
       <c r="B46" s="0">
         <v>0.2990754213683402</v>
@@ -580,7 +583,7 @@
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>-0.014659460612705691</v>
+        <v>0.0046788658355207896</v>
       </c>
       <c r="B48" s="0">
         <v>-0.020480319618094621</v>
@@ -591,7 +594,7 @@
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>0.31945894642461042</v>
+        <v>0.31995824901507114</v>
       </c>
       <c r="B49" s="0">
         <v>0.31889287265194305</v>
@@ -613,7 +616,7 @@
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>-0.016453321281413427</v>
+        <v>0.0051688167929343463</v>
       </c>
       <c r="B51" s="0">
         <v>-0.023176773630162736</v>
@@ -624,7 +627,7 @@
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>0.33937115873981372</v>
+        <v>0.33995253104366951</v>
       </c>
       <c r="B52" s="0">
         <v>0.3386880211920536</v>
@@ -646,7 +649,7 @@
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>-0.018325763615001014</v>
+        <v>0.0056697914376085306</v>
       </c>
       <c r="B54" s="0">
         <v>-0.026032352720070363</v>
@@ -657,7 +660,7 @@
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>0.35927589338852084</v>
+        <v>0.35994655172565365</v>
       </c>
       <c r="B55" s="0">
         <v>0.35845902156159937</v>
@@ -679,7 +682,7 @@
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>-0.020276091093393782</v>
+        <v>0.0061810904195572927</v>
       </c>
       <c r="B57" s="0">
         <v>-0.029050593893449269</v>
@@ -690,7 +693,7 @@
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>0.37917284016516595</v>
+        <v>0.37994032177636933</v>
       </c>
       <c r="B58" s="0">
         <v>0.37820376160591584</v>
@@ -712,7 +715,7 @@
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>-0.022304328431130768</v>
+        <v>0.006702098183261015</v>
       </c>
       <c r="B60" s="0">
         <v>-0.032236103799952565</v>
@@ -723,7 +726,7 @@
     </row>
     <row r="61">
       <c r="A61" s="0">
-        <v>0.39906161194198236</v>
+        <v>0.39993385131379067</v>
       </c>
       <c r="B61" s="0">
         <v>0.39791981925336101</v>
@@ -745,7 +748,7 @@
     </row>
     <row r="63">
       <c r="A63" s="0">
-        <v>-0.024411220420257337</v>
+        <v>0.0072322555379183652</v>
       </c>
       <c r="B63" s="0">
         <v>-0.035594570807750608</v>
@@ -756,7 +759,7 @@
     </row>
     <row r="64">
       <c r="A64" s="0">
-        <v>0.41894173285978631</v>
+        <v>0.41992715037654027</v>
       </c>
       <c r="B64" s="0">
         <v>0.41760441476609428</v>
@@ -778,7 +781,7 @@
     </row>
     <row r="66">
       <c r="A66" s="0">
-        <v>-0.026598233849039209</v>
+        <v>0.0077710347405684057</v>
       </c>
       <c r="B66" s="0">
         <v>-0.03913278022907709</v>
@@ -789,7 +792,7 @@
     </row>
     <row r="67">
       <c r="A67" s="0">
-        <v>0.43881262568756579</v>
+        <v>0.43992022946935172</v>
       </c>
       <c r="B67" s="0">
         <v>0.4372543574699263</v>
@@ -811,7 +814,7 @@
     </row>
     <row r="69">
       <c r="A69" s="0">
-        <v>-0.028867562461433252</v>
+        <v>0.0083179159811449608</v>
       </c>
       <c r="B69" s="0">
         <v>-0.042858632386706799</v>
@@ -822,7 +825,7 @@
     </row>
     <row r="70">
       <c r="A70" s="0">
-        <v>0.45867359799982099</v>
+        <v>0.45991310015158693</v>
       </c>
       <c r="B70" s="0">
         <v>0.4568659859266252</v>
@@ -844,7 +847,7 @@
     </row>
     <row r="72">
       <c r="A72" s="0">
-        <v>-0.031222134924985177</v>
+        <v>0.0088723642209960398</v>
       </c>
       <c r="B72" s="0">
         <v>-0.046781163137155461</v>
@@ -855,7 +858,7 @@
     </row>
     <row r="73">
       <c r="A73" s="0">
-        <v>0.47852382680314975</v>
+        <v>0.479905775687682</v>
       </c>
       <c r="B73" s="0">
         <v>0.47643510042380177</v>
@@ -877,7 +880,7 @@
     </row>
     <row r="75">
       <c r="A75" s="0">
-        <v>-0.033665625775684153</v>
+        <v>0.0094338053521087137</v>
       </c>
       <c r="B75" s="0">
         <v>-0.050910566373012091</v>
@@ -888,7 +891,7 @@
     </row>
     <row r="76">
       <c r="A76" s="0">
-        <v>0.49836234121906942</v>
+        <v>0.49989827178114837</v>
       </c>
       <c r="B76" s="0">
         <v>0.49595688655709186</v>
@@ -910,7 +913,7 @@
     </row>
     <row r="78">
       <c r="A78" s="0">
-        <v>-0.036202469306639042</v>
+        <v>0.010001600613914157</v>
       </c>
       <c r="B78" s="0">
         <v>-0.055258217909738547</v>
@@ -921,7 +924,7 @@
     </row>
     <row r="79">
       <c r="A79" s="0">
-        <v>0.5181880027982575</v>
+        <v>0.51989060741600757</v>
       </c>
       <c r="B79" s="0">
         <v>0.51542582856784969</v>
@@ -943,7 +946,7 @@
     </row>
     <row r="81">
       <c r="A81" s="0">
-        <v>-0.038837876362503507</v>
+        <v>0.010575018126738845</v>
       </c>
       <c r="B81" s="0">
         <v>-0.059836700016323893</v>
@@ -954,7 +957,7 @@
     </row>
     <row r="82">
       <c r="A82" s="0">
-        <v>0.5379994830019188</v>
+        <v>0.53988280583099546</v>
       </c>
       <c r="B82" s="0">
         <v>0.53483561097863674</v>
@@ -976,7 +979,7 @@
     </row>
     <row r="84">
       <c r="A84" s="0">
-        <v>-0.041577853992483649</v>
+        <v>0.011153200272224995</v>
       </c>
       <c r="B84" s="0">
         <v>-0.064659825668289553</v>
@@ -987,7 +990,7 @@
     </row>
     <row r="85">
       <c r="A85" s="0">
-        <v>0.55779523733842773</v>
+        <v>0.55987489565185555</v>
       </c>
       <c r="B85" s="0">
         <v>0.55417900694102673</v>
@@ -1009,7 +1012,7 @@
     </row>
     <row r="87">
       <c r="A87" s="0">
-        <v>-0.044429227900455184</v>
+        <v>0.011735125465595434</v>
       </c>
       <c r="B87" s="0">
         <v>-0.069742661378605991</v>
@@ -1020,7 +1023,7 @@
     </row>
     <row r="88">
       <c r="A88" s="0">
-        <v>0.57757347558726091</v>
+        <v>0.57986691220432629</v>
       </c>
       <c r="B88" s="0">
         <v>0.57344775157950523</v>
@@ -1042,7 +1045,7 @@
     </row>
     <row r="90">
       <c r="A90" s="0">
-        <v>-0.047399667609922744</v>
+        <v>0.012319562614175328</v>
       </c>
       <c r="B90" s="0">
         <v>-0.075101547188861834</v>
@@ -1053,7 +1056,7 @@
     </row>
     <row r="91">
       <c r="A91" s="0">
-        <v>0.59733212747701492</v>
+        <v>0.5998588990229573</v>
       </c>
       <c r="B91" s="0">
         <v>0.59263239848707139</v>
@@ -1075,7 +1078,7 @@
     </row>
     <row r="93">
       <c r="A93" s="0">
-        <v>-0.050497714232725206</v>
+        <v>0.012905016229881178</v>
       </c>
       <c r="B93" s="0">
         <v>-0.08075411207003684</v>
@@ -1086,7 +1089,7 @@
     </row>
     <row r="94">
       <c r="A94" s="0">
-        <v>0.61706880310943857</v>
+        <v>0.61985090955529687</v>
       </c>
       <c r="B94" s="0">
         <v>0.61172215741040148</v>
@@ -1108,7 +1111,7 @@
     </row>
     <row r="96">
       <c r="A96" s="0">
-        <v>-0.053732810691651742</v>
+        <v>0.013489659745802849</v>
       </c>
       <c r="B96" s="0">
         <v>-0.086719282578696641</v>
@@ -1119,7 +1122,7 @@
     </row>
     <row r="97">
       <c r="A97" s="0">
-        <v>0.63678074733642598</v>
+        <v>0.63984300903196145</v>
       </c>
       <c r="B97" s="0">
         <v>0.63070471106593406</v>
@@ -1141,7 +1144,7 @@
     </row>
     <row r="99">
       <c r="A99" s="0">
-        <v>-0.057115334196208192</v>
+        <v>0.014071254059820612</v>
       </c>
       <c r="B99" s="0">
         <v>-0.093017282128303805</v>
@@ -1152,7 +1155,7 @@
     </row>
     <row r="100">
       <c r="A100" s="0">
-        <v>0.65646478720133972</v>
+        <v>0.65983527642218476</v>
       </c>
       <c r="B100" s="0">
         <v>0.64956600896770167</v>
@@ -1174,7 +1177,7 @@
     </row>
     <row r="102">
       <c r="A102" s="0">
-        <v>-0.060656630704903715</v>
+        <v>0.014647047667795883</v>
       </c>
       <c r="B102" s="0">
         <v>-0.099669617653454404</v>
@@ -1185,7 +1188,7 @@
     </row>
     <row r="103">
       <c r="A103" s="0">
-        <v>0.67611727144963685</v>
+        <v>0.67982780630849993</v>
       </c>
       <c r="B103" s="0">
         <v>0.66829003614288074</v>
@@ -1207,7 +1210,7 @@
     </row>
     <row r="105">
       <c r="A105" s="0">
-        <v>-0.064369051023285703</v>
+        <v>0.015213653925700402</v>
       </c>
       <c r="B105" s="0">
         <v>-0.10669904975323694</v>
@@ -1218,7 +1221,7 @@
     </row>
     <row r="106">
       <c r="A106" s="0">
-        <v>0.69573400099649962</v>
+        <v>0.69982071037271587</v>
       </c>
       <c r="B106" s="0">
         <v>0.68685855468783352</v>
@@ -1240,7 +1243,7 @@
     </row>
     <row r="108">
       <c r="A108" s="0">
-        <v>-0.068265988080530055</v>
+        <v>0.015766899957368023</v>
       </c>
       <c r="B108" s="0">
         <v>-0.11412954158440533</v>
@@ -1251,7 +1254,7 @@
     </row>
     <row r="109">
       <c r="A109" s="0">
-        <v>0.7153101491114231</v>
+        <v>0.7198141179565607</v>
       </c>
       <c r="B109" s="0">
         <v>0.70525081630972519</v>
@@ -1273,7 +1276,7 @@
     </row>
     <row r="111">
       <c r="A111" s="0">
-        <v>-0.072361914793896254</v>
+        <v>0.01630164045696484</v>
       </c>
       <c r="B111" s="0">
         <v>-0.12198618082230504</v>
@@ -1284,7 +1287,7 @@
     </row>
     <row r="112">
       <c r="A112" s="0">
-        <v>0.7348401699424153</v>
+        <v>0.73980817479519001</v>
       </c>
       <c r="B112" s="0">
         <v>0.72344324435003604</v>
@@ -1306,7 +1309,7 @@
     </row>
     <row r="114">
       <c r="A114" s="0">
-        <v>-0.076672421764065399</v>
+        <v>0.01681152806702611</v>
       </c>
       <c r="B114" s="0">
         <v>-0.13029506790648593</v>
@@ -1317,7 +1320,7 @@
     </row>
     <row r="115">
       <c r="A115" s="0">
-        <v>0.75431769385739511</v>
+        <v>0.75980303844460018</v>
       </c>
       <c r="B115" s="0">
         <v>0.74140908435142305</v>
@@ -1339,7 +1342,7 @@
     </row>
     <row r="117">
       <c r="A117" s="0">
-        <v>-0.08121425383853248</v>
+        <v>0.01728873007613246</v>
       </c>
       <c r="B117" s="0">
         <v>-0.13908316253234382</v>
@@ -1350,7 +1353,7 @@
     </row>
     <row r="118">
       <c r="A118" s="0">
-        <v>0.77373540793039641</v>
+        <v>0.77979886801858467</v>
       </c>
       <c r="B118" s="0">
         <v>0.7591180230768434</v>
@@ -1372,7 +1375,7 @@
     </row>
     <row r="120">
       <c r="A120" s="0">
-        <v>-0.086005344326873151</v>
+        <v>0.017723578793439481</v>
       </c>
       <c r="B120" s="0">
         <v>-0.14837807894158248</v>
@@ -1383,7 +1386,7 @@
     </row>
     <row r="121">
       <c r="A121" s="0">
-        <v>0.79308491974973694</v>
+        <v>0.79979580443883058</v>
       </c>
       <c r="B121" s="0">
         <v>0.77653577710337895</v>
@@ -1405,7 +1408,7 @@
     </row>
     <row r="123">
       <c r="A123" s="0">
-        <v>-0.091064845341612008</v>
+        <v>0.01810414002438342</v>
       </c>
       <c r="B123" s="0">
         <v>-0.15820781901700645</v>
@@ -1416,7 +1419,7 @@
     </row>
     <row r="124">
       <c r="A124" s="0">
-        <v>0.8123566025808624</v>
+        <v>0.81979393520974508</v>
       </c>
       <c r="B124" s="0">
         <v>0.79362365379304978</v>
@@ -1438,7 +1441,7 @@
     </row>
     <row r="126">
       <c r="A126" s="0">
-        <v>-0.096413152360956295</v>
+        <v>0.018415680484108535</v>
       </c>
       <c r="B126" s="0">
         <v>-0.16860043053422838</v>
@@ -1449,7 +1452,7 @@
     </row>
     <row r="127">
       <c r="A127" s="0">
-        <v>0.83153941978732027</v>
+        <v>0.83979323433963082</v>
       </c>
       <c r="B127" s="0">
         <v>0.81033808970602761</v>
@@ -1471,7 +1474,7 @@
     </row>
     <row r="129">
       <c r="A129" s="0">
-        <v>-0.10207192065278624</v>
+        <v>0.018640010627159458</v>
       </c>
       <c r="B129" s="0">
         <v>-0.17958357622452514</v>
@@ -1482,7 +1485,7 @@
     </row>
     <row r="130">
       <c r="A130" s="0">
-        <v>0.850620726312041</v>
+        <v>0.85979346280382929</v>
       </c>
       <c r="B130" s="0">
         <v>0.82663017449989851</v>
@@ -1504,7 +1507,7 @@
     </row>
     <row r="132">
       <c r="A132" s="0">
-        <v>-0.10806407064962807</v>
+        <v>0.018754674138618792</v>
       </c>
       <c r="B132" s="0">
         <v>-0.19118399765724936</v>
@@ -1515,7 +1518,7 @@
     </row>
     <row r="133">
       <c r="A133" s="0">
-        <v>0.86958604496514547</v>
+        <v>0.87979400691193788</v>
       </c>
       <c r="B133" s="0">
         <v>0.84244517219374759</v>
@@ -1537,7 +1540,7 @@
     </row>
     <row r="135">
       <c r="A135" s="0">
-        <v>-0.11441377870737503</v>
+        <v>0.018731949165536704</v>
       </c>
       <c r="B135" s="0">
         <v>-0.20342685650560333</v>
@@ -1548,7 +1551,7 @@
     </row>
     <row r="136">
       <c r="A136" s="0">
-        <v>0.88841881527711142</v>
+        <v>0.8997936196259666</v>
       </c>
       <c r="B136" s="0">
         <v>0.85772205650982547</v>
@@ -1570,7 +1573,7 @@
     </row>
     <row r="138">
       <c r="A138" s="0">
-        <v>-0.12114644890109756</v>
+        <v>0.01853761933592199</v>
       </c>
       <c r="B138" s="0">
         <v>-0.21633493473102702</v>
@@ -1581,7 +1584,7 @@
     </row>
     <row r="139">
       <c r="A139" s="0">
-        <v>0.9071001127878906</v>
+        <v>0.91979001105365155</v>
       </c>
       <c r="B139" s="0">
         <v>0.87239308296396589</v>
@@ -1603,7 +1606,7 @@
     </row>
     <row r="141">
       <c r="A141" s="0">
-        <v>-0.12828866059437791</v>
+        <v>0.018129465064807206</v>
       </c>
       <c r="B141" s="0">
         <v>-0.22992767490681559</v>
@@ -1614,7 +1617,7 @@
     </row>
     <row r="142">
       <c r="A142" s="0">
-        <v>0.92560833689323574</v>
+        <v>0.93977920567652906</v>
       </c>
       <c r="B142" s="0">
         <v>0.88638342754185395</v>
@@ -1636,7 +1639,7 @@
     </row>
     <row r="144">
       <c r="A144" s="0">
-        <v>-0.13586808545062387</v>
+        <v>0.017455418518494869</v>
       </c>
       <c r="B144" s="0">
         <v>-0.24422004269867625</v>
@@ -1647,7 +1650,7 @@
     </row>
     <row r="145">
       <c r="A145" s="0">
-        <v>0.94391886580986351</v>
+        <v>0.95975454043038821</v>
       </c>
       <c r="B145" s="0">
         <v>0.89961093017408567</v>
@@ -1669,7 +1672,7 @@
     </row>
     <row r="147">
       <c r="A147" s="0">
-        <v>-0.14391336632558699</v>
+        <v>0.016451321007359018</v>
       </c>
       <c r="B147" s="0">
         <v>-0.25922119594031773</v>
@@ -1680,7 +1683,7 @@
     </row>
     <row r="148">
       <c r="A148" s="0">
-        <v>0.96200367791518127</v>
+        <v>0.97970511237447111</v>
       </c>
       <c r="B148" s="0">
         <v>0.91198599067734964</v>
@@ -1702,7 +1705,7 @@
     </row>
     <row r="150">
       <c r="A150" s="0">
-        <v>-0.15245394908595064</v>
+        <v>0.01503822389546162</v>
       </c>
       <c r="B150" s="0">
         <v>-0.27493294941687119</v>
@@ -1713,7 +1716,7 @@
     </row>
     <row r="151">
       <c r="A151" s="0">
-        <v>0.97983093974438551</v>
+        <v>0.99961338731416638</v>
       </c>
       <c r="B151" s="0">
         <v>0.92341167502774724</v>
@@ -1735,7 +1738,7 @@
     </row>
     <row r="153">
       <c r="A153" s="0">
-        <v>-0.1615198568459128</v>
+        <v>0.013119192093683009</v>
       </c>
       <c r="B153" s="0">
         <v>-0.29134803213847932</v>

</xml_diff>

<commit_message>
Lots of changes to structure to only calculate the asked external forces need to modify linesearch method accordingly
</commit_message>
<xml_diff>
--- a/experiments/pneunet/quarter_circle_with_gravity.xlsx
+++ b/experiments/pneunet/quarter_circle_with_gravity.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -52,16 +52,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C203"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="16.42578125" customWidth="true"/>
-    <col min="2" max="2" width="16.42578125" customWidth="true"/>
     <col min="1" max="1" width="15.7109375" customWidth="true"/>
+    <col min="2" max="2" width="15.7109375" customWidth="true"/>
+    <col min="3" max="3" width="15.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -135,10 +132,10 @@
         <v>0.040000393448394019</v>
       </c>
       <c r="B7" s="0">
-        <v>0.039998641669755503</v>
+        <v>0.040000393606201612</v>
       </c>
       <c r="C7" s="0">
-        <v>0.039997767266149668</v>
+        <v>0.040000393766434057</v>
       </c>
     </row>
     <row r="8">
@@ -154,13 +151,13 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>8.0904185094077174e-05</v>
+        <v>8.0904185094082514e-05</v>
       </c>
       <c r="B9" s="0">
-        <v>-0.00023783135019860396</v>
+        <v>8.0865159776113244e-05</v>
       </c>
       <c r="C9" s="0">
-        <v>-0.00030255222421157426</v>
+        <v>8.0825515520115731e-05</v>
       </c>
     </row>
     <row r="10">
@@ -168,10 +165,10 @@
         <v>0.060000402724620663</v>
       </c>
       <c r="B10" s="0">
-        <v>0.059993361105477691</v>
+        <v>0.060000403466886384</v>
       </c>
       <c r="C10" s="0">
-        <v>0.059989069200822649</v>
+        <v>0.060000404220626469</v>
       </c>
     </row>
     <row r="11">
@@ -187,24 +184,24 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>0.00022893671078018558</v>
+        <v>0.00022893671078020155</v>
       </c>
       <c r="B12" s="0">
-        <v>-0.00069981678168456985</v>
+        <v>0.00022881869715464656</v>
       </c>
       <c r="C12" s="0">
-        <v>-0.00089423182861944747</v>
+        <v>0.00022869879838457836</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>0.079999919458515353</v>
+        <v>0.079999919458515339</v>
       </c>
       <c r="B13" s="0">
-        <v>0.079982063047464275</v>
+        <v>0.079999921444093527</v>
       </c>
       <c r="C13" s="0">
-        <v>0.079970237185987697</v>
+        <v>0.079999923460476061</v>
       </c>
     </row>
     <row r="14">
@@ -220,24 +217,24 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>0.0004329364119163195</v>
+        <v>0.00043293641191635094</v>
       </c>
       <c r="B15" s="0">
-        <v>-0.0013736367375571123</v>
+        <v>0.00043269646785639294</v>
       </c>
       <c r="C15" s="0">
-        <v>-0.0017632353838712756</v>
+        <v>0.00043245266829246005</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>0.099998902518024999</v>
+        <v>0.099998902518024985</v>
       </c>
       <c r="B16" s="0">
-        <v>0.099962984829389853</v>
+        <v>0.09999890663503988</v>
       </c>
       <c r="C16" s="0">
-        <v>0.099937998877414488</v>
+        <v>0.099998910816029324</v>
       </c>
     </row>
     <row r="17">
@@ -253,13 +250,13 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>0.00068385998607482616</v>
+        <v>0.00068385998607487723</v>
       </c>
       <c r="B18" s="0">
-        <v>-0.0022482827383885399</v>
+        <v>0.00068345010267297098</v>
       </c>
       <c r="C18" s="0">
-        <v>-0.0028993414089715256</v>
+        <v>0.00068303360112872058</v>
       </c>
     </row>
     <row r="19">
@@ -267,10 +264,10 @@
         <v>0.11999734958525113</v>
       </c>
       <c r="B19" s="0">
-        <v>0.11993462621331887</v>
+        <v>0.11999735697348765</v>
       </c>
       <c r="C19" s="0">
-        <v>0.11988937792597402</v>
+        <v>0.11999736447651163</v>
       </c>
     </row>
     <row r="20">
@@ -286,13 +283,13 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>0.00097437919335646695</v>
+        <v>0.00097437919335654089</v>
       </c>
       <c r="B21" s="0">
-        <v>-0.0033140139524611241</v>
+        <v>0.00097374403889801482</v>
       </c>
       <c r="C21" s="0">
-        <v>-0.0042938735303691931</v>
+        <v>0.00097309858800060105</v>
       </c>
     </row>
     <row r="22">
@@ -300,10 +297,10 @@
         <v>0.13999527941231149</v>
       </c>
       <c r="B22" s="0">
-        <v>0.13989568786878934</v>
+        <v>0.13999529150703682</v>
       </c>
       <c r="C22" s="0">
-        <v>0.1398216033687685</v>
+        <v>0.1399953037893206</v>
       </c>
     </row>
     <row r="23">
@@ -319,13 +316,13 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>0.001298554321017023</v>
+        <v>0.001298554321017121</v>
       </c>
       <c r="B24" s="0">
-        <v>-0.0045623173694999478</v>
+        <v>0.0012976286966938767</v>
       </c>
       <c r="C24" s="0">
-        <v>-0.0059396669319342014</v>
+        <v>0.0012966880178314347</v>
       </c>
     </row>
     <row r="25">
@@ -333,10 +330,10 @@
         <v>0.15999272093643743</v>
       </c>
       <c r="B25" s="0">
-        <v>0.1598450171128547</v>
+        <v>0.15999273953276055</v>
       </c>
       <c r="C25" s="0">
-        <v>0.1597320267945799</v>
+        <v>0.15999275841642743</v>
       </c>
     </row>
     <row r="26">
@@ -352,13 +349,13 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>0.0016515694584630218</v>
+        <v>0.001651569458463143</v>
       </c>
       <c r="B27" s="0">
-        <v>-0.0059858718565799496</v>
+        <v>0.0016502753396330876</v>
       </c>
       <c r="C27" s="0">
-        <v>-0.0078310385654583262</v>
+        <v>0.0016489601161611515</v>
       </c>
     </row>
     <row r="28">
@@ -366,10 +363,10 @@
         <v>0.17998970677200701</v>
       </c>
       <c r="B28" s="0">
-        <v>0.17978155966307771</v>
+        <v>0.17998973411107483</v>
       </c>
       <c r="C28" s="0">
-        <v>0.1796180455232215</v>
+        <v>0.17998976187027876</v>
       </c>
     </row>
     <row r="29">
@@ -385,13 +382,13 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>0.0020295178313289712</v>
+        <v>0.0020295178313291112</v>
       </c>
       <c r="B30" s="0">
-        <v>-0.0075785162816909436</v>
+        <v>0.002027760853991784</v>
       </c>
       <c r="C30" s="0">
-        <v>-0.0099637614309225596</v>
+        <v>0.0020259751602299128</v>
       </c>
     </row>
     <row r="31">
@@ -399,10 +396,10 @@
         <v>0.19998626947172521</v>
       </c>
       <c r="B31" s="0">
-        <v>0.19970431627180585</v>
+        <v>0.19998630835184442</v>
       </c>
       <c r="C31" s="0">
-        <v>0.19947703015030882</v>
+        <v>0.19998634782499186</v>
       </c>
     </row>
     <row r="32">
@@ -418,24 +415,24 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>0.0024292276486627255</v>
+        <v>0.0024292276486628773</v>
       </c>
       <c r="B33" s="0">
-        <v>-0.0093352218184543541</v>
+        <v>0.0024268928789572884</v>
       </c>
       <c r="C33" s="0">
-        <v>-0.012335043102301666</v>
+        <v>0.0024245198801960961</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>0.21998243951985058</v>
+        <v>0.21998243951985055</v>
       </c>
       <c r="B34" s="0">
-        <v>0.21961230320829944</v>
+        <v>0.21998249343728207</v>
       </c>
       <c r="C34" s="0">
-        <v>0.21930625489760067</v>
+        <v>0.21998254816903717</v>
       </c>
     </row>
     <row r="35">
@@ -451,13 +448,13 @@
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>0.0028481207103325779</v>
+        <v>0.0028481207103327306</v>
       </c>
       <c r="B36" s="0">
-        <v>-0.011252068489995014</v>
+        <v>0.0028450675047790234</v>
       </c>
       <c r="C36" s="0">
-        <v>-0.01494350856068782</v>
+        <v>0.002841964232896667</v>
       </c>
     </row>
     <row r="37">
@@ -465,10 +462,10 @@
         <v>0.23997824439218543</v>
       </c>
       <c r="B37" s="0">
-        <v>0.23950451563620795</v>
+        <v>0.23997831771806113</v>
       </c>
       <c r="C37" s="0">
-        <v>0.23910282927463575</v>
+        <v>0.23997839213749173</v>
       </c>
     </row>
     <row r="38">
@@ -484,13 +481,13 @@
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>0.0032840974759685551</v>
+        <v>0.0032840974759686956</v>
       </c>
       <c r="B39" s="0">
-        <v>-0.013326225967040032</v>
+        <v>0.0032801532008669221</v>
       </c>
       <c r="C39" s="0">
-        <v>-0.017789187295421598</v>
+        <v>0.0032761441701844034</v>
       </c>
     </row>
     <row r="40">
@@ -498,10 +495,10 @@
         <v>0.2599737082593247</v>
       </c>
       <c r="B40" s="0">
-        <v>0.25937989299829051</v>
+        <v>0.25997380646102136</v>
       </c>
       <c r="C40" s="0">
-        <v>0.25886362960040205</v>
+        <v>0.25997390610405385</v>
       </c>
     </row>
     <row r="41">
@@ -517,13 +514,13 @@
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>0.0037354434734995414</v>
+        <v>0.0037354434734996529</v>
       </c>
       <c r="B42" s="0">
-        <v>-0.015555938601613809</v>
+        <v>0.003730395801846211</v>
       </c>
       <c r="C42" s="0">
-        <v>-0.020873504539756296</v>
+        <v>0.0037252651789658935</v>
       </c>
     </row>
     <row r="43">
@@ -531,10 +528,10 @@
         <v>0.27996885206651662</v>
       </c>
       <c r="B43" s="0">
-        <v>0.27923728556890853</v>
+        <v>0.27996898198400172</v>
       </c>
       <c r="C43" s="0">
-        <v>0.27858522895489007</v>
+        <v>0.27996911377040934</v>
       </c>
     </row>
     <row r="44">
@@ -550,13 +547,13 @@
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>0.0042007528753908296</v>
+        <v>0.0042007528753908929</v>
       </c>
       <c r="B45" s="0">
-        <v>-0.017940514650365533</v>
+        <v>0.004194340316794741</v>
       </c>
       <c r="C45" s="0">
-        <v>-0.024199276414790472</v>
+        <v>0.0041878222942388832</v>
       </c>
     </row>
     <row r="46">
@@ -564,10 +561,10 @@
         <v>0.29996369382498672</v>
       </c>
       <c r="B46" s="0">
-        <v>0.2990754213683402</v>
+        <v>0.29996386401522607</v>
       </c>
       <c r="C46" s="0">
-        <v>0.29826382413040553</v>
+        <v>0.29996403659275089</v>
       </c>
     </row>
     <row r="47">
@@ -583,13 +580,13 @@
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>0.0046788658355207896</v>
+        <v>0.0046788658355207836</v>
       </c>
       <c r="B48" s="0">
-        <v>-0.020480319618094621</v>
+        <v>0.0046707660761850563</v>
       </c>
       <c r="C48" s="0">
-        <v>-0.027770708658621295</v>
+        <v>0.0046625330199226997</v>
       </c>
     </row>
     <row r="49">
@@ -597,10 +594,10 @@
         <v>0.31995824901507114</v>
       </c>
       <c r="B49" s="0">
-        <v>0.31889287265194305</v>
+        <v>0.31995847018065637</v>
       </c>
       <c r="C49" s="0">
-        <v>0.3178951581324192</v>
+        <v>0.3199586943516135</v>
       </c>
     </row>
     <row r="50">
@@ -616,13 +613,13 @@
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>0.0051688167929343463</v>
+        <v>0.0051688167929342423</v>
       </c>
       <c r="B51" s="0">
-        <v>-0.023176773630162736</v>
+        <v>0.0051586323253718612</v>
       </c>
       <c r="C51" s="0">
-        <v>-0.031593398511536988</v>
+        <v>0.0051482801672973469</v>
       </c>
     </row>
     <row r="52">
@@ -630,10 +627,10 @@
         <v>0.33995253104366951</v>
       </c>
       <c r="B52" s="0">
-        <v>0.3386880211920536</v>
+        <v>0.33995281656547338</v>
       </c>
       <c r="C52" s="0">
-        <v>0.33747443674069888</v>
+        <v>0.33995310581433319</v>
       </c>
     </row>
     <row r="53">
@@ -649,24 +646,24 @@
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>0.0056697914376085306</v>
+        <v>0.0056697914376082964</v>
       </c>
       <c r="B54" s="0">
-        <v>-0.026032352720070363</v>
+        <v>0.0056570318390741677</v>
       </c>
       <c r="C54" s="0">
-        <v>-0.035674339207031544</v>
+        <v>0.0056440620627998175</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>0.35994655172565365</v>
+        <v>0.35994655172565371</v>
       </c>
       <c r="B55" s="0">
-        <v>0.35845902156159937</v>
+        <v>0.35994691832363146</v>
       </c>
       <c r="C55" s="0">
-        <v>0.35699623758501825</v>
+        <v>0.35994728946759769</v>
       </c>
     </row>
     <row r="56">
@@ -682,13 +679,13 @@
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>0.0061810904195572927</v>
+        <v>0.0061810904195568868</v>
       </c>
       <c r="B57" s="0">
-        <v>-0.029050593893449269</v>
+        <v>0.0061651504888468487</v>
       </c>
       <c r="C57" s="0">
-        <v>-0.040021926376570191</v>
+        <v>0.0061489479053449302</v>
       </c>
     </row>
     <row r="58">
@@ -696,10 +693,10 @@
         <v>0.37994032177636933</v>
       </c>
       <c r="B58" s="0">
-        <v>0.37820376160591584</v>
+        <v>0.37994079032764755</v>
       </c>
       <c r="C58" s="0">
-        <v>0.37645441011785696</v>
+        <v>0.37994126431604508</v>
       </c>
     </row>
     <row r="59">
@@ -715,13 +712,13 @@
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>0.006702098183261015</v>
+        <v>0.0067020981832603879</v>
       </c>
       <c r="B60" s="0">
-        <v>-0.032236103799952565</v>
+        <v>0.0066822309609053734</v>
       </c>
       <c r="C60" s="0">
-        <v>-0.044645965506890602</v>
+        <v>0.0066620362828176778</v>
       </c>
     </row>
     <row r="61">
@@ -729,10 +726,10 @@
         <v>0.39993385131379067</v>
       </c>
       <c r="B61" s="0">
-        <v>0.39791981925336101</v>
+        <v>0.39993444786291737</v>
       </c>
       <c r="C61" s="0">
-        <v>0.39584196478190409</v>
+        <v>0.39993505075503616</v>
       </c>
     </row>
     <row r="62">
@@ -748,24 +745,24 @@
     </row>
     <row r="63">
       <c r="A63" s="0">
-        <v>0.0072322555379183652</v>
+        <v>0.0072322555379174544</v>
       </c>
       <c r="B63" s="0">
-        <v>-0.035594570807750608</v>
+        <v>0.007207539006664143</v>
       </c>
       <c r="C63" s="0">
-        <v>-0.049557679385005361</v>
+        <v>0.0071824149981166924</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0">
-        <v>0.41992715037654027</v>
+        <v>0.41992715037654033</v>
       </c>
       <c r="B64" s="0">
-        <v>0.41760441476609428</v>
+        <v>0.41992790737911401</v>
       </c>
       <c r="C64" s="0">
-        <v>0.41515094957654236</v>
+        <v>0.41992867153355928</v>
       </c>
     </row>
     <row r="65">
@@ -781,13 +778,13 @@
     </row>
     <row r="66">
       <c r="A66" s="0">
-        <v>0.0077710347405684057</v>
+        <v>0.007771034740567141</v>
       </c>
       <c r="B66" s="0">
-        <v>-0.03913278022907709</v>
+        <v>0.007740330721205088</v>
       </c>
       <c r="C66" s="0">
-        <v>-0.05476971421991076</v>
+        <v>0.0077091204133600691</v>
       </c>
     </row>
     <row r="67">
@@ -795,10 +792,10 @@
         <v>0.43992022946935172</v>
       </c>
       <c r="B67" s="0">
-        <v>0.4372543574699263</v>
+        <v>0.43992118731692875</v>
       </c>
       <c r="C67" s="0">
-        <v>0.43437231212988453</v>
+        <v>0.43992215282768538</v>
       </c>
     </row>
     <row r="68">
@@ -814,13 +811,13 @@
     </row>
     <row r="69">
       <c r="A69" s="0">
-        <v>0.0083179159811449608</v>
+        <v>0.008317915981143259</v>
       </c>
       <c r="B69" s="0">
-        <v>-0.042858632386706799</v>
+        <v>0.0082798193906272848</v>
       </c>
       <c r="C69" s="0">
-        <v>-0.060296142832222809</v>
+        <v>0.0082410944991633452</v>
       </c>
     </row>
     <row r="70">
@@ -828,10 +825,10 @@
         <v>0.45991310015158693</v>
       </c>
       <c r="B70" s="0">
-        <v>0.4568659859266252</v>
+        <v>0.4599143090322233</v>
       </c>
       <c r="C70" s="0">
-        <v>0.45349574528829589</v>
+        <v>0.45991552544613312</v>
       </c>
     </row>
     <row r="71">
@@ -847,24 +844,24 @@
     </row>
     <row r="72">
       <c r="A72" s="0">
-        <v>0.0088723642209960398</v>
+        <v>0.0088723642209938072</v>
       </c>
       <c r="B72" s="0">
-        <v>-0.046781163137155461</v>
+        <v>0.0088251404298631854</v>
       </c>
       <c r="C72" s="0">
-        <v>-0.066152462943357623</v>
+        <v>0.0087771376732617007</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0">
-        <v>0.479905775687682</v>
+        <v>0.47990577568768206</v>
       </c>
       <c r="B73" s="0">
-        <v>0.47643510042380177</v>
+        <v>0.47990729784165348</v>
       </c>
       <c r="C73" s="0">
-        <v>0.47250951415307091</v>
+        <v>0.47990882618650405</v>
       </c>
     </row>
     <row r="74">
@@ -880,24 +877,24 @@
     </row>
     <row r="75">
       <c r="A75" s="0">
-        <v>0.0094338053521087137</v>
+        <v>0.0094338053521058479</v>
       </c>
       <c r="B75" s="0">
-        <v>-0.050910566373012091</v>
+        <v>0.0093753128471970783</v>
       </c>
       <c r="C75" s="0">
-        <v>-0.072355588163096077</v>
+        <v>0.0093158553245503966</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0">
-        <v>0.49989827178114837</v>
+        <v>0.49989827178114843</v>
       </c>
       <c r="B76" s="0">
-        <v>0.49595688655709186</v>
+        <v>0.49990018421348958</v>
       </c>
       <c r="C76" s="0">
-        <v>0.49140026243670665</v>
+        <v>0.49990209935161456</v>
       </c>
     </row>
     <row r="77">
@@ -913,24 +910,24 @@
     </row>
     <row r="78">
       <c r="A78" s="0">
-        <v>0.010001600613914157</v>
+        <v>0.01000160061391055</v>
       </c>
       <c r="B78" s="0">
-        <v>-0.055258217909738547</v>
+        <v>0.0099291955165490033</v>
       </c>
       <c r="C78" s="0">
-        <v>-0.078923828755966749</v>
+        <v>0.0098555956364018097</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0">
-        <v>0.51989060741600757</v>
+        <v>0.51989060741600768</v>
       </c>
       <c r="B79" s="0">
-        <v>0.51542582856784969</v>
+        <v>0.51989300512345171</v>
       </c>
       <c r="C79" s="0">
-        <v>0.51015279599591257</v>
+        <v>0.51989539841657517</v>
       </c>
     </row>
     <row r="80">
@@ -946,24 +943,24 @@
     </row>
     <row r="81">
       <c r="A81" s="0">
-        <v>0.010575018126738845</v>
+        <v>0.010575018126734387</v>
       </c>
       <c r="B81" s="0">
-        <v>-0.059836700016323893</v>
+        <v>0.010485436306627776</v>
       </c>
       <c r="C81" s="0">
-        <v>-0.085876858649496526</v>
+        <v>0.010394375934212023</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0">
-        <v>0.53988280583099546</v>
+        <v>0.53988280583099557</v>
       </c>
       <c r="B82" s="0">
-        <v>0.53483561097863674</v>
+        <v>0.53988580558565391</v>
       </c>
       <c r="C82" s="0">
-        <v>0.52874984144737136</v>
+        <v>0.53988878780303606</v>
       </c>
     </row>
     <row r="83">
@@ -979,24 +976,24 @@
     </row>
     <row r="84">
       <c r="A84" s="0">
-        <v>0.011153200272224995</v>
+        <v>0.011153200272219584</v>
       </c>
       <c r="B84" s="0">
-        <v>-0.064659825668289553</v>
+        <v>0.011042411796904088</v>
       </c>
       <c r="C84" s="0">
-        <v>-0.09323566441718692</v>
+        <v>0.010929794269081174</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0">
-        <v>0.55987489565185555</v>
+        <v>0.55987489565185566</v>
       </c>
       <c r="B85" s="0">
-        <v>0.55417900694102673</v>
+        <v>0.55987864034943258</v>
       </c>
       <c r="C85" s="0">
-        <v>0.54717177791432192</v>
+        <v>0.55988234465806208</v>
       </c>
     </row>
     <row r="86">
@@ -1012,24 +1009,24 @@
     </row>
     <row r="87">
       <c r="A87" s="0">
-        <v>0.011735125465595434</v>
+        <v>0.011735125465588973</v>
       </c>
       <c r="B87" s="0">
-        <v>-0.069742661378605991</v>
+        <v>0.011598154889692543</v>
       </c>
       <c r="C87" s="0">
-        <v>-0.10102247111251393</v>
+        <v>0.011458922289332435</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0">
-        <v>0.57986691220432629</v>
+        <v>0.57986691220432651</v>
       </c>
       <c r="B88" s="0">
-        <v>0.57344775157950523</v>
+        <v>0.57987157571790393</v>
       </c>
       <c r="C88" s="0">
-        <v>0.5653963402246498</v>
+        <v>0.57987616043687495</v>
       </c>
     </row>
     <row r="89">
@@ -1045,24 +1042,24 @@
     </row>
     <row r="90">
       <c r="A90" s="0">
-        <v>0.012319562614175328</v>
+        <v>0.012319562614167728</v>
       </c>
       <c r="B90" s="0">
-        <v>-0.075101547188861834</v>
+        <v>0.012150267086595914</v>
       </c>
       <c r="C90" s="0">
-        <v>-0.10926063883520842</v>
+        <v>0.011978174614666402</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0">
-        <v>0.5998588990229573</v>
+        <v>0.59985889902295753</v>
       </c>
       <c r="B91" s="0">
-        <v>0.59263239848707139</v>
+        <v>0.59986469138399456</v>
       </c>
       <c r="C91" s="0">
-        <v>0.58339829233186624</v>
+        <v>0.59987034192856303</v>
       </c>
     </row>
     <row r="92">
@@ -1078,24 +1075,24 @@
     </row>
     <row r="93">
       <c r="A93" s="0">
-        <v>0.012905016229881178</v>
+        <v>0.012905016229872366</v>
       </c>
       <c r="B93" s="0">
-        <v>-0.08075411207003684</v>
+        <v>0.01269581151191067</v>
       </c>
       <c r="C93" s="0">
-        <v>-0.1179745227687037</v>
+        <v>0.012483148876778897</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0">
-        <v>0.61985090955529687</v>
+        <v>0.6198509095552972</v>
       </c>
       <c r="B94" s="0">
-        <v>0.61172215741040148</v>
+        <v>0.61985808207952076</v>
       </c>
       <c r="C94" s="0">
-        <v>0.60114907041872534</v>
+        <v>0.61986501110671832</v>
       </c>
     </row>
     <row r="95">
@@ -1111,24 +1108,24 @@
     </row>
     <row r="96">
       <c r="A96" s="0">
-        <v>0.013489659745802849</v>
+        <v>0.013489659745792772</v>
       </c>
       <c r="B96" s="0">
-        <v>-0.086719282578696641</v>
+        <v>0.013231181904644387</v>
       </c>
       <c r="C96" s="0">
-        <v>-0.12718928813499028</v>
+        <v>0.01296842927860957</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0">
-        <v>0.63984300903196145</v>
+        <v>0.63984300903196178</v>
       </c>
       <c r="B97" s="0">
-        <v>0.63070471106593406</v>
+        <v>0.63985185866945926</v>
       </c>
       <c r="C97" s="0">
-        <v>0.61861639614280794</v>
+        <v>0.63986030277867456</v>
       </c>
     </row>
     <row r="98">
@@ -1144,24 +1141,24 @@
     </row>
     <row r="99">
       <c r="A99" s="0">
-        <v>0.014071254059820612</v>
+        <v>0.014071254059809248</v>
       </c>
       <c r="B99" s="0">
-        <v>-0.093017282128303805</v>
+        <v>0.013751941726162582</v>
       </c>
       <c r="C99" s="0">
-        <v>-0.13693067007691834</v>
+        <v>0.013427344894437808</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0">
-        <v>0.65983527642218476</v>
+        <v>0.65983527642218509</v>
       </c>
       <c r="B100" s="0">
-        <v>0.64956600896770167</v>
+        <v>0.65984614806096387</v>
       </c>
       <c r="C100" s="0">
-        <v>0.63576386188324496</v>
+        <v>0.6598563583642123</v>
       </c>
     </row>
     <row r="101">
@@ -1177,24 +1174,24 @@
     </row>
     <row r="102">
       <c r="A102" s="0">
-        <v>0.014647047667795883</v>
+        <v>0.014647047667783237</v>
       </c>
       <c r="B102" s="0">
-        <v>-0.099669617653454404</v>
+        <v>0.014252626194538832</v>
       </c>
       <c r="C102" s="0">
-        <v>-0.14722466691977812</v>
+        <v>0.013851671914492212</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0">
-        <v>0.67982780630849993</v>
+        <v>0.67982780630850037</v>
       </c>
       <c r="B103" s="0">
-        <v>0.66829003614288074</v>
+        <v>0.67984109087954536</v>
       </c>
       <c r="C103" s="0">
-        <v>0.65255049175325941</v>
+        <v>0.67985331312915609</v>
       </c>
     </row>
     <row r="104">
@@ -1210,24 +1207,24 @@
     </row>
     <row r="105">
       <c r="A105" s="0">
-        <v>0.015213653925700402</v>
+        <v>0.015213653925686505</v>
       </c>
       <c r="B105" s="0">
-        <v>-0.10669904975323694</v>
+        <v>0.014726498400858894</v>
       </c>
       <c r="C105" s="0">
-        <v>-0.15809715362709542</v>
+        <v>0.014231266546115316</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0">
-        <v>0.69982071037271587</v>
+        <v>0.6998207103727162</v>
       </c>
       <c r="B106" s="0">
-        <v>0.68685855468783352</v>
+        <v>0.69983683520787054</v>
       </c>
       <c r="C106" s="0">
-        <v>0.66893028467559168</v>
+        <v>0.69985127263474045</v>
       </c>
     </row>
     <row r="107">
@@ -1243,24 +1240,24 @@
     </row>
     <row r="108">
       <c r="A108" s="0">
-        <v>0.015766899957368023</v>
+        <v>0.01576689995735293</v>
       </c>
       <c r="B108" s="0">
-        <v>-0.11412954158440533</v>
+        <v>0.015165248615771103</v>
       </c>
       <c r="C108" s="0">
-        <v>-0.16957340062411438</v>
+        <v>0.014553612219786554</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0">
-        <v>0.7198141179565607</v>
+        <v>0.71981411795656114</v>
       </c>
       <c r="B109" s="0">
-        <v>0.70525081630972519</v>
+        <v>0.71983352365482745</v>
       </c>
       <c r="C109" s="0">
-        <v>0.68485174911121005</v>
+        <v>0.71985027173902305</v>
       </c>
     </row>
     <row r="110">
@@ -1276,24 +1273,24 @@
     </row>
     <row r="111">
       <c r="A111" s="0">
-        <v>0.01630164045696484</v>
+        <v>0.016301640456948627</v>
       </c>
       <c r="B111" s="0">
-        <v>-0.12198618082230504</v>
+        <v>0.015558623371124762</v>
       </c>
       <c r="C111" s="0">
-        <v>-0.18167748163271172</v>
+        <v>0.014803261001075336</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0">
-        <v>0.73980817479519001</v>
+        <v>0.73980817479519057</v>
       </c>
       <c r="B112" s="0">
-        <v>0.72344324435003604</v>
+        <v>0.73983126942289379</v>
       </c>
       <c r="C112" s="0">
-        <v>0.70025744322634509</v>
+        <v>0.73985020574194071</v>
       </c>
     </row>
     <row r="113">
@@ -1309,24 +1306,24 @@
     </row>
     <row r="114">
       <c r="A114" s="0">
-        <v>0.01681152806702611</v>
+        <v>0.016811528067008863</v>
       </c>
       <c r="B114" s="0">
-        <v>-0.13029506790648593</v>
+        <v>0.015893967801849655</v>
       </c>
       <c r="C114" s="0">
-        <v>-0.19443155291576564</v>
+        <v>0.014961144563169758</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0">
-        <v>0.75980303844460018</v>
+        <v>0.75980303844460062</v>
       </c>
       <c r="B115" s="0">
-        <v>0.74140908435142305</v>
+        <v>0.75983011456274496</v>
       </c>
       <c r="C115" s="0">
-        <v>0.71508353951332326</v>
+        <v>0.75985071749881139</v>
       </c>
     </row>
     <row r="116">
@@ -1342,24 +1339,24 @@
     </row>
     <row r="117">
       <c r="A117" s="0">
-        <v>0.01728873007613246</v>
+        <v>0.017288730076114277</v>
       </c>
       <c r="B117" s="0">
-        <v>-0.13908316253234382</v>
+        <v>0.016155660945650269</v>
       </c>
       <c r="C117" s="0">
-        <v>-0.20785498561139379</v>
+        <v>0.015003724628962281</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0">
-        <v>0.77979886801858467</v>
+        <v>0.77979886801858511</v>
       </c>
       <c r="B118" s="0">
-        <v>0.7591180230768434</v>
+        <v>0.77982995977506531</v>
       </c>
       <c r="C118" s="0">
-        <v>0.72925943925564907</v>
+        <v>0.77985101546966129</v>
       </c>
     </row>
     <row r="119">
@@ -1375,24 +1372,24 @@
     </row>
     <row r="120">
       <c r="A120" s="0">
-        <v>0.017723578793439481</v>
+        <v>0.017723578793420468</v>
       </c>
       <c r="B120" s="0">
-        <v>-0.14837807894158248</v>
+        <v>0.016324419107588403</v>
       </c>
       <c r="C120" s="0">
-        <v>-0.22196333298077089</v>
+        <v>0.014901946406324175</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0">
-        <v>0.79979580443883058</v>
+        <v>0.79979580443883103</v>
       </c>
       <c r="B121" s="0">
-        <v>0.77653577710337895</v>
+        <v>0.79983044922315349</v>
       </c>
       <c r="C121" s="0">
-        <v>0.74270746980007418</v>
+        <v>0.79984958410317175</v>
       </c>
     </row>
     <row r="122">
@@ -1408,24 +1405,24 @@
     </row>
     <row r="123">
       <c r="A123" s="0">
-        <v>0.01810414002438342</v>
+        <v>0.018104140024363679</v>
       </c>
       <c r="B123" s="0">
-        <v>-0.15820781901700645</v>
+        <v>0.016376436905807788</v>
       </c>
       <c r="C123" s="0">
-        <v>-0.23676711583476212</v>
+        <v>0.014619951325119245</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0">
-        <v>0.81979393520974508</v>
+        <v>0.81979393520974564</v>
       </c>
       <c r="B124" s="0">
-        <v>0.79362365379304978</v>
+        <v>0.81983078476433069</v>
       </c>
       <c r="C124" s="0">
-        <v>0.75534270632138079</v>
+        <v>0.81984372722963794</v>
       </c>
     </row>
     <row r="125">
@@ -1441,24 +1438,24 @@
     </row>
     <row r="126">
       <c r="A126" s="0">
-        <v>0.018415680484108535</v>
+        <v>0.018415680484088166</v>
       </c>
       <c r="B126" s="0">
-        <v>-0.16860043053422838</v>
+        <v>0.016282329189638546</v>
       </c>
       <c r="C126" s="0">
-        <v>-0.25227041269720801</v>
+        <v>0.014113497781238478</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0">
-        <v>0.83979323433963082</v>
+        <v>0.83979323433963138</v>
       </c>
       <c r="B127" s="0">
-        <v>0.81033808970602761</v>
+        <v>0.83982943013834943</v>
       </c>
       <c r="C127" s="0">
-        <v>0.76707296943455816</v>
+        <v>0.83982885359983173</v>
       </c>
     </row>
     <row r="128">
@@ -1474,24 +1471,24 @@
     </row>
     <row r="129">
       <c r="A129" s="0">
-        <v>0.018640010627159458</v>
+        <v>0.018640010627138548</v>
       </c>
       <c r="B129" s="0">
-        <v>-0.17958357622452514</v>
+        <v>0.016005829786276266</v>
       </c>
       <c r="C129" s="0">
-        <v>-0.26846924707515674</v>
+        <v>0.013328031727982624</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0">
-        <v>0.85979346280382929</v>
+        <v>0.85979346280382984</v>
       </c>
       <c r="B130" s="0">
-        <v>0.82663017449989851</v>
+        <v>0.85982364447203474</v>
       </c>
       <c r="C130" s="0">
-        <v>0.77779906018622846</v>
+        <v>0.8597973659564806</v>
       </c>
     </row>
     <row r="131">
@@ -1507,24 +1504,24 @@
     </row>
     <row r="132">
       <c r="A132" s="0">
-        <v>0.018754674138618792</v>
+        <v>0.018754674138597424</v>
       </c>
       <c r="B132" s="0">
-        <v>-0.19118399765724936</v>
+        <v>0.015502195457511794</v>
       </c>
       <c r="C132" s="0">
-        <v>-0.28534977330454181</v>
+        <v>0.01219634531761747</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0">
-        <v>0.87979400691193788</v>
+        <v>0.87979400691193843</v>
       </c>
       <c r="B133" s="0">
-        <v>0.84244517219374759</v>
+        <v>0.87980875224254507</v>
       </c>
       <c r="C133" s="0">
-        <v>0.78741530388334091</v>
+        <v>0.8797369432617328</v>
       </c>
     </row>
     <row r="134">
@@ -1540,24 +1537,24 @@
     </row>
     <row r="135">
       <c r="A135" s="0">
-        <v>0.018731949165536704</v>
+        <v>0.018731949165514947</v>
       </c>
       <c r="B135" s="0">
-        <v>-0.20342685650560333</v>
+        <v>0.014716256716367337</v>
       </c>
       <c r="C135" s="0">
-        <v>-0.30288627563724407</v>
+        <v>0.010635766518204949</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0">
-        <v>0.8997936196259666</v>
+        <v>0.89979361962596704</v>
       </c>
       <c r="B136" s="0">
-        <v>0.85772205650982547</v>
+        <v>0.89977700809019068</v>
       </c>
       <c r="C136" s="0">
-        <v>0.79581048271720578</v>
+        <v>0.89962789907042084</v>
       </c>
     </row>
     <row r="137">
@@ -1573,24 +1570,24 @@
     </row>
     <row r="138">
       <c r="A138" s="0">
-        <v>0.01853761933592199</v>
+        <v>0.0185376193358999</v>
       </c>
       <c r="B138" s="0">
-        <v>-0.21633493473102702</v>
+        <v>0.013580053861364461</v>
       </c>
       <c r="C138" s="0">
-        <v>-0.32103901329898182</v>
+        <v>0.0085448458701047978</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0">
-        <v>0.91979001105365155</v>
+        <v>0.91979001105365199</v>
       </c>
       <c r="B139" s="0">
-        <v>0.87239308296396589</v>
+        <v>0.91971584166338505</v>
       </c>
       <c r="C139" s="0">
-        <v>0.8028692425401931</v>
+        <v>0.91943914342900568</v>
       </c>
     </row>
     <row r="140">
@@ -1606,24 +1603,24 @@
     </row>
     <row r="141">
       <c r="A141" s="0">
-        <v>0.018129465064807206</v>
+        <v>0.018129465064784831</v>
       </c>
       <c r="B141" s="0">
-        <v>-0.22992767490681559</v>
+        <v>0.012010002066295239</v>
       </c>
       <c r="C141" s="0">
-        <v>-0.33975196774349148</v>
+        <v>0.0057995678251975555</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0">
-        <v>0.93977920567652906</v>
+        <v>0.93977920567652962</v>
       </c>
       <c r="B142" s="0">
-        <v>0.88638342754185395</v>
+        <v>0.93960515902888042</v>
       </c>
       <c r="C142" s="0">
-        <v>0.80847405923101701</v>
+        <v>0.93912205528298143</v>
       </c>
     </row>
     <row r="143">
@@ -1639,24 +1636,24 @@
     </row>
     <row r="144">
       <c r="A144" s="0">
-        <v>0.017455418518494869</v>
+        <v>0.017455418518472241</v>
       </c>
       <c r="B144" s="0">
-        <v>-0.24422004269867625</v>
+        <v>0.0099035541404343778</v>
       </c>
       <c r="C144" s="0">
-        <v>-0.35895057739786429</v>
+        <v>0.0022492499917515676</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0">
-        <v>0.95975454043038821</v>
+        <v>0.95975454043038877</v>
       </c>
       <c r="B145" s="0">
-        <v>0.89961093017408567</v>
+        <v>0.95941321891923614</v>
       </c>
       <c r="C145" s="0">
-        <v>0.81250784211105254</v>
+        <v>0.95860127612295221</v>
       </c>
     </row>
     <row r="146">
@@ -1672,24 +1669,24 @@
     </row>
     <row r="147">
       <c r="A147" s="0">
-        <v>0.016451321007359018</v>
+        <v>0.016451321007336168</v>
       </c>
       <c r="B147" s="0">
-        <v>-0.25922119594031773</v>
+        <v>0.0071353938281108935</v>
       </c>
       <c r="C147" s="0">
-        <v>-0.37853957925305048</v>
+        <v>-0.002287429394063038</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0">
-        <v>0.97970511237447111</v>
+        <v>0.97970511237447155</v>
       </c>
       <c r="B148" s="0">
-        <v>0.91198599067734964</v>
+        <v>0.97909037858866332</v>
       </c>
       <c r="C148" s="0">
-        <v>0.81485723277199784</v>
+        <v>0.97776107578404214</v>
       </c>
     </row>
     <row r="149">
@@ -1705,24 +1702,24 @@
     </row>
     <row r="150">
       <c r="A150" s="0">
-        <v>0.01503822389546162</v>
+        <v>0.015038223895438557</v>
       </c>
       <c r="B150" s="0">
-        <v>-0.27493294941687119</v>
+        <v>0.0035533339473565518</v>
       </c>
       <c r="C150" s="0">
-        <v>-0.39840111403823814</v>
+        <v>-0.0080253010082360667</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0">
-        <v>0.99961338731416638</v>
+        <v>0.99961338731416682</v>
       </c>
       <c r="B151" s="0">
-        <v>0.92341167502774724</v>
+        <v>0.99855970511617509</v>
       </c>
       <c r="C151" s="0">
-        <v>0.81541662438072182</v>
+        <v>0.99642559974648048</v>
       </c>
     </row>
     <row r="152">
@@ -1738,13 +1735,13 @@
     </row>
     <row r="153">
       <c r="A153" s="0">
-        <v>0.013119192093683009</v>
+        <v>0.013119192093659747</v>
       </c>
       <c r="B153" s="0">
-        <v>-0.29134803213847932</v>
+        <v>-0.0010256193421931642</v>
       </c>
       <c r="C153" s="0">
-        <v>-0.41839328931791631</v>
+        <v>-0.015212513281316351</v>
       </c>
     </row>
     <row r="154">

</xml_diff>